<commit_message>
change continue show/gt N to dict parameter
</commit_message>
<xml_diff>
--- a/doc/特征工程流程图v2.1.xlsx
+++ b/doc/特征工程流程图v2.1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{CFE9F7F5-109F-4310-BCEF-7CCAAFDCC890}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{4C5A50FD-D2BB-4C84-86DE-6ECC87CBCD58}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5580" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="824" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3760,8 +3760,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42112F6E-780D-4F54-AA89-CB41E0B2B8FB}">
   <dimension ref="B2:M132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F50" sqref="F50"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20:B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -6110,23 +6110,23 @@
       </c>
       <c r="D4">
         <f ca="1">FLOOR(RAND()*10,1)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E4">
         <f ca="1">FLOOR(RAND()*1000,1)</f>
-        <v>294</v>
+        <v>325</v>
       </c>
       <c r="F4">
         <f t="shared" ref="F4:H19" ca="1" si="0">FLOOR(RAND()*1000,1)</f>
-        <v>234</v>
+        <v>177</v>
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="0"/>
-        <v>86</v>
+        <v>600</v>
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="0"/>
-        <v>17</v>
+        <v>430</v>
       </c>
       <c r="I4" t="s">
         <v>133</v>
@@ -6144,23 +6144,23 @@
       </c>
       <c r="D5">
         <f t="shared" ref="D5:D68" ca="1" si="1">FLOOR(RAND()*10,1)</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E5">
         <f t="shared" ref="E5:H68" ca="1" si="2">FLOOR(RAND()*1000,1)</f>
-        <v>536</v>
+        <v>563</v>
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="0"/>
-        <v>168</v>
+        <v>678</v>
       </c>
       <c r="G5">
         <f t="shared" ca="1" si="0"/>
-        <v>422</v>
+        <v>764</v>
       </c>
       <c r="H5">
         <f t="shared" ca="1" si="0"/>
-        <v>339</v>
+        <v>676</v>
       </c>
       <c r="I5" t="s">
         <v>134</v>
@@ -6178,23 +6178,23 @@
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="2"/>
-        <v>810</v>
+        <v>528</v>
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="0"/>
-        <v>728</v>
+        <v>276</v>
       </c>
       <c r="G6">
         <f t="shared" ca="1" si="0"/>
-        <v>822</v>
+        <v>289</v>
       </c>
       <c r="H6">
         <f t="shared" ca="1" si="0"/>
-        <v>73</v>
+        <v>457</v>
       </c>
       <c r="I6" t="s">
         <v>134</v>
@@ -6212,23 +6212,23 @@
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="2"/>
-        <v>928</v>
+        <v>163</v>
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="0"/>
-        <v>88</v>
+        <v>611</v>
       </c>
       <c r="G7">
         <f t="shared" ca="1" si="0"/>
-        <v>833</v>
+        <v>143</v>
       </c>
       <c r="H7">
         <f t="shared" ca="1" si="0"/>
-        <v>272</v>
+        <v>871</v>
       </c>
       <c r="I7" t="s">
         <v>135</v>
@@ -6246,23 +6246,23 @@
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="2"/>
-        <v>661</v>
+        <v>33</v>
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="0"/>
-        <v>135</v>
+        <v>156</v>
       </c>
       <c r="G8">
         <f t="shared" ca="1" si="0"/>
-        <v>548</v>
+        <v>950</v>
       </c>
       <c r="H8">
         <f t="shared" ca="1" si="0"/>
-        <v>316</v>
+        <v>697</v>
       </c>
       <c r="I8" t="s">
         <v>134</v>
@@ -6280,23 +6280,23 @@
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="2"/>
-        <v>487</v>
+        <v>476</v>
       </c>
       <c r="F9">
         <f t="shared" ca="1" si="0"/>
-        <v>657</v>
+        <v>226</v>
       </c>
       <c r="G9">
         <f t="shared" ca="1" si="0"/>
-        <v>61</v>
+        <v>879</v>
       </c>
       <c r="H9">
         <f t="shared" ca="1" si="0"/>
-        <v>454</v>
+        <v>940</v>
       </c>
       <c r="I9" t="s">
         <v>134</v>
@@ -6314,23 +6314,23 @@
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="2"/>
-        <v>266</v>
+        <v>76</v>
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="0"/>
-        <v>418</v>
+        <v>871</v>
       </c>
       <c r="G10">
         <f t="shared" ca="1" si="0"/>
-        <v>469</v>
+        <v>210</v>
       </c>
       <c r="H10">
         <f t="shared" ca="1" si="0"/>
-        <v>855</v>
+        <v>333</v>
       </c>
       <c r="I10" t="s">
         <v>134</v>
@@ -6348,23 +6348,23 @@
       </c>
       <c r="D11">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="2"/>
-        <v>564</v>
+        <v>643</v>
       </c>
       <c r="F11">
         <f t="shared" ca="1" si="0"/>
-        <v>470</v>
+        <v>983</v>
       </c>
       <c r="G11">
         <f t="shared" ca="1" si="0"/>
-        <v>228</v>
+        <v>250</v>
       </c>
       <c r="H11">
         <f t="shared" ca="1" si="0"/>
-        <v>216</v>
+        <v>31</v>
       </c>
       <c r="I11" t="s">
         <v>135</v>
@@ -6382,23 +6382,23 @@
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="2"/>
-        <v>715</v>
+        <v>334</v>
       </c>
       <c r="F12">
         <f t="shared" ca="1" si="0"/>
-        <v>687</v>
+        <v>509</v>
       </c>
       <c r="G12">
         <f t="shared" ca="1" si="0"/>
-        <v>354</v>
+        <v>322</v>
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="0"/>
-        <v>151</v>
+        <v>914</v>
       </c>
       <c r="I12" t="s">
         <v>134</v>
@@ -6416,23 +6416,23 @@
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="2"/>
-        <v>208</v>
+        <v>891</v>
       </c>
       <c r="F13">
         <f t="shared" ca="1" si="0"/>
-        <v>459</v>
+        <v>247</v>
       </c>
       <c r="G13">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>815</v>
       </c>
       <c r="H13">
         <f t="shared" ca="1" si="0"/>
-        <v>15</v>
+        <v>131</v>
       </c>
       <c r="I13" t="s">
         <v>134</v>
@@ -6450,23 +6450,23 @@
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="2"/>
-        <v>893</v>
+        <v>156</v>
       </c>
       <c r="F14">
         <f t="shared" ca="1" si="0"/>
-        <v>787</v>
+        <v>222</v>
       </c>
       <c r="G14">
         <f t="shared" ca="1" si="0"/>
-        <v>964</v>
+        <v>249</v>
       </c>
       <c r="H14">
         <f t="shared" ca="1" si="0"/>
-        <v>950</v>
+        <v>671</v>
       </c>
       <c r="I14" t="s">
         <v>134</v>
@@ -6484,23 +6484,23 @@
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="2"/>
-        <v>296</v>
+        <v>677</v>
       </c>
       <c r="F15">
         <f t="shared" ca="1" si="0"/>
-        <v>240</v>
+        <v>80</v>
       </c>
       <c r="G15">
         <f t="shared" ca="1" si="0"/>
-        <v>171</v>
+        <v>593</v>
       </c>
       <c r="H15">
         <f t="shared" ca="1" si="0"/>
-        <v>788</v>
+        <v>31</v>
       </c>
       <c r="I15" t="s">
         <v>134</v>
@@ -6518,19 +6518,19 @@
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="2"/>
-        <v>923</v>
+        <v>453</v>
       </c>
       <c r="F16">
         <f t="shared" ca="1" si="0"/>
-        <v>213</v>
+        <v>345</v>
       </c>
       <c r="G16">
         <f t="shared" ca="1" si="0"/>
-        <v>54</v>
+        <v>432</v>
       </c>
       <c r="H16">
         <f t="shared" ca="1" si="0"/>
-        <v>133</v>
+        <v>653</v>
       </c>
       <c r="I16" t="s">
         <v>134</v>
@@ -6548,23 +6548,23 @@
       </c>
       <c r="D17">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="2"/>
-        <v>859</v>
+        <v>488</v>
       </c>
       <c r="F17">
         <f t="shared" ca="1" si="0"/>
-        <v>964</v>
+        <v>45</v>
       </c>
       <c r="G17">
         <f t="shared" ca="1" si="0"/>
-        <v>486</v>
+        <v>61</v>
       </c>
       <c r="H17">
         <f t="shared" ca="1" si="0"/>
-        <v>479</v>
+        <v>176</v>
       </c>
       <c r="I17" t="s">
         <v>133</v>
@@ -6582,23 +6582,23 @@
       </c>
       <c r="D18">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E18">
         <f t="shared" ca="1" si="2"/>
-        <v>872</v>
+        <v>422</v>
       </c>
       <c r="F18">
         <f t="shared" ca="1" si="0"/>
-        <v>762</v>
+        <v>650</v>
       </c>
       <c r="G18">
         <f t="shared" ca="1" si="0"/>
-        <v>972</v>
+        <v>886</v>
       </c>
       <c r="H18">
         <f t="shared" ca="1" si="0"/>
-        <v>376</v>
+        <v>173</v>
       </c>
       <c r="I18" t="s">
         <v>134</v>
@@ -6616,23 +6616,23 @@
       </c>
       <c r="D19">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E19">
         <f t="shared" ca="1" si="2"/>
-        <v>964</v>
+        <v>821</v>
       </c>
       <c r="F19">
         <f t="shared" ca="1" si="0"/>
-        <v>267</v>
+        <v>96</v>
       </c>
       <c r="G19">
         <f t="shared" ca="1" si="0"/>
-        <v>297</v>
+        <v>947</v>
       </c>
       <c r="H19">
         <f t="shared" ca="1" si="0"/>
-        <v>533</v>
+        <v>388</v>
       </c>
       <c r="I19" t="s">
         <v>134</v>
@@ -6650,23 +6650,23 @@
       </c>
       <c r="D20">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E20">
         <f t="shared" ca="1" si="2"/>
-        <v>46</v>
+        <v>239</v>
       </c>
       <c r="F20">
         <f t="shared" ca="1" si="2"/>
-        <v>821</v>
+        <v>496</v>
       </c>
       <c r="G20">
         <f t="shared" ca="1" si="2"/>
-        <v>388</v>
+        <v>783</v>
       </c>
       <c r="H20">
         <f t="shared" ca="1" si="2"/>
-        <v>395</v>
+        <v>468</v>
       </c>
       <c r="I20" t="s">
         <v>134</v>
@@ -6684,23 +6684,23 @@
       </c>
       <c r="D21">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E21">
         <f t="shared" ca="1" si="2"/>
-        <v>679</v>
+        <v>933</v>
       </c>
       <c r="F21">
         <f t="shared" ca="1" si="2"/>
-        <v>221</v>
+        <v>383</v>
       </c>
       <c r="G21">
         <f t="shared" ca="1" si="2"/>
-        <v>868</v>
+        <v>115</v>
       </c>
       <c r="H21">
         <f t="shared" ca="1" si="2"/>
-        <v>357</v>
+        <v>698</v>
       </c>
       <c r="I21" t="s">
         <v>134</v>
@@ -6722,19 +6722,19 @@
       </c>
       <c r="E22">
         <f t="shared" ca="1" si="2"/>
-        <v>978</v>
+        <v>161</v>
       </c>
       <c r="F22">
         <f t="shared" ca="1" si="2"/>
-        <v>44</v>
+        <v>659</v>
       </c>
       <c r="G22">
         <f t="shared" ca="1" si="2"/>
-        <v>585</v>
+        <v>301</v>
       </c>
       <c r="H22">
         <f t="shared" ca="1" si="2"/>
-        <v>685</v>
+        <v>378</v>
       </c>
       <c r="I22" t="s">
         <v>133</v>
@@ -6752,23 +6752,23 @@
       </c>
       <c r="D23">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E23">
         <f t="shared" ca="1" si="2"/>
-        <v>326</v>
+        <v>550</v>
       </c>
       <c r="F23">
         <f t="shared" ca="1" si="2"/>
-        <v>704</v>
+        <v>452</v>
       </c>
       <c r="G23">
         <f t="shared" ca="1" si="2"/>
-        <v>571</v>
+        <v>655</v>
       </c>
       <c r="H23">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>636</v>
       </c>
       <c r="I23" t="s">
         <v>135</v>
@@ -6786,23 +6786,23 @@
       </c>
       <c r="D24">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E24">
         <f t="shared" ca="1" si="2"/>
-        <v>982</v>
+        <v>727</v>
       </c>
       <c r="F24">
         <f t="shared" ca="1" si="2"/>
-        <v>506</v>
+        <v>220</v>
       </c>
       <c r="G24">
         <f t="shared" ca="1" si="2"/>
-        <v>48</v>
+        <v>232</v>
       </c>
       <c r="H24">
         <f t="shared" ca="1" si="2"/>
-        <v>824</v>
+        <v>891</v>
       </c>
       <c r="I24" t="s">
         <v>134</v>
@@ -6820,23 +6820,23 @@
       </c>
       <c r="D25">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E25">
         <f t="shared" ca="1" si="2"/>
-        <v>572</v>
+        <v>934</v>
       </c>
       <c r="F25">
         <f t="shared" ca="1" si="2"/>
-        <v>933</v>
+        <v>702</v>
       </c>
       <c r="G25">
         <f t="shared" ca="1" si="2"/>
-        <v>99</v>
+        <v>884</v>
       </c>
       <c r="H25">
         <f t="shared" ca="1" si="2"/>
-        <v>805</v>
+        <v>279</v>
       </c>
       <c r="I25" t="s">
         <v>133</v>
@@ -6854,23 +6854,23 @@
       </c>
       <c r="D26">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E26">
         <f t="shared" ca="1" si="2"/>
-        <v>781</v>
+        <v>968</v>
       </c>
       <c r="F26">
         <f t="shared" ca="1" si="2"/>
-        <v>455</v>
+        <v>131</v>
       </c>
       <c r="G26">
         <f t="shared" ca="1" si="2"/>
-        <v>728</v>
+        <v>549</v>
       </c>
       <c r="H26">
         <f t="shared" ca="1" si="2"/>
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="I26" t="s">
         <v>134</v>
@@ -6888,23 +6888,23 @@
       </c>
       <c r="D27">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E27">
         <f t="shared" ca="1" si="2"/>
-        <v>900</v>
+        <v>530</v>
       </c>
       <c r="F27">
         <f t="shared" ca="1" si="2"/>
-        <v>917</v>
+        <v>285</v>
       </c>
       <c r="G27">
         <f t="shared" ca="1" si="2"/>
-        <v>456</v>
+        <v>34</v>
       </c>
       <c r="H27">
         <f t="shared" ca="1" si="2"/>
-        <v>372</v>
+        <v>226</v>
       </c>
       <c r="I27" t="s">
         <v>133</v>
@@ -6922,23 +6922,23 @@
       </c>
       <c r="D28">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E28">
         <f t="shared" ca="1" si="2"/>
-        <v>288</v>
+        <v>338</v>
       </c>
       <c r="F28">
         <f t="shared" ca="1" si="2"/>
-        <v>56</v>
+        <v>755</v>
       </c>
       <c r="G28">
         <f t="shared" ca="1" si="2"/>
-        <v>605</v>
+        <v>246</v>
       </c>
       <c r="H28">
         <f t="shared" ca="1" si="2"/>
-        <v>551</v>
+        <v>882</v>
       </c>
       <c r="I28" t="s">
         <v>133</v>
@@ -6956,19 +6956,19 @@
       </c>
       <c r="D29">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E29">
         <f t="shared" ca="1" si="2"/>
-        <v>622</v>
+        <v>959</v>
       </c>
       <c r="F29">
         <f t="shared" ca="1" si="2"/>
-        <v>918</v>
+        <v>113</v>
       </c>
       <c r="H29">
         <f t="shared" ca="1" si="2"/>
-        <v>130</v>
+        <v>814</v>
       </c>
       <c r="I29" t="s">
         <v>135</v>
@@ -6986,23 +6986,23 @@
       </c>
       <c r="D30">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="E30">
         <f t="shared" ca="1" si="2"/>
-        <v>757</v>
+        <v>514</v>
       </c>
       <c r="F30">
         <f t="shared" ca="1" si="2"/>
-        <v>195</v>
+        <v>795</v>
       </c>
       <c r="G30">
         <f t="shared" ca="1" si="2"/>
-        <v>684</v>
+        <v>761</v>
       </c>
       <c r="H30">
         <f t="shared" ca="1" si="2"/>
-        <v>465</v>
+        <v>371</v>
       </c>
       <c r="I30" t="s">
         <v>133</v>
@@ -7020,23 +7020,23 @@
       </c>
       <c r="D31">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E31">
         <f t="shared" ca="1" si="2"/>
-        <v>842</v>
+        <v>92</v>
       </c>
       <c r="F31">
         <f t="shared" ca="1" si="2"/>
-        <v>253</v>
+        <v>311</v>
       </c>
       <c r="G31">
         <f t="shared" ca="1" si="2"/>
-        <v>94</v>
+        <v>203</v>
       </c>
       <c r="H31">
         <f t="shared" ca="1" si="2"/>
-        <v>768</v>
+        <v>593</v>
       </c>
       <c r="I31" t="s">
         <v>133</v>
@@ -7054,23 +7054,23 @@
       </c>
       <c r="D32">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E32">
         <f t="shared" ca="1" si="2"/>
-        <v>212</v>
+        <v>646</v>
       </c>
       <c r="F32">
         <f t="shared" ca="1" si="2"/>
-        <v>568</v>
+        <v>327</v>
       </c>
       <c r="G32">
         <f t="shared" ca="1" si="2"/>
-        <v>830</v>
+        <v>843</v>
       </c>
       <c r="H32">
         <f t="shared" ca="1" si="2"/>
-        <v>732</v>
+        <v>109</v>
       </c>
       <c r="I32" t="s">
         <v>135</v>
@@ -7088,23 +7088,23 @@
       </c>
       <c r="D33">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E33">
         <f t="shared" ca="1" si="2"/>
-        <v>979</v>
+        <v>988</v>
       </c>
       <c r="F33">
         <f t="shared" ca="1" si="2"/>
-        <v>639</v>
+        <v>841</v>
       </c>
       <c r="G33">
         <f t="shared" ca="1" si="2"/>
-        <v>40</v>
+        <v>506</v>
       </c>
       <c r="H33">
         <f t="shared" ca="1" si="2"/>
-        <v>471</v>
+        <v>18</v>
       </c>
       <c r="I33" t="s">
         <v>134</v>
@@ -7122,23 +7122,23 @@
       </c>
       <c r="D34">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E34">
         <f t="shared" ca="1" si="2"/>
-        <v>347</v>
+        <v>229</v>
       </c>
       <c r="F34">
         <f t="shared" ca="1" si="2"/>
-        <v>288</v>
+        <v>365</v>
       </c>
       <c r="G34">
         <f t="shared" ca="1" si="2"/>
-        <v>599</v>
+        <v>328</v>
       </c>
       <c r="H34">
         <f t="shared" ca="1" si="2"/>
-        <v>569</v>
+        <v>501</v>
       </c>
       <c r="I34" t="s">
         <v>134</v>
@@ -7160,19 +7160,19 @@
       </c>
       <c r="E35">
         <f t="shared" ca="1" si="2"/>
-        <v>873</v>
+        <v>368</v>
       </c>
       <c r="F35">
         <f t="shared" ca="1" si="2"/>
-        <v>71</v>
+        <v>320</v>
       </c>
       <c r="G35">
         <f t="shared" ca="1" si="2"/>
-        <v>819</v>
+        <v>944</v>
       </c>
       <c r="H35">
         <f t="shared" ca="1" si="2"/>
-        <v>473</v>
+        <v>661</v>
       </c>
       <c r="I35" t="s">
         <v>134</v>
@@ -7190,23 +7190,23 @@
       </c>
       <c r="D36">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E36">
         <f t="shared" ca="1" si="2"/>
-        <v>132</v>
+        <v>264</v>
       </c>
       <c r="F36">
         <f t="shared" ca="1" si="2"/>
-        <v>502</v>
+        <v>869</v>
       </c>
       <c r="G36">
         <f t="shared" ca="1" si="2"/>
-        <v>557</v>
+        <v>450</v>
       </c>
       <c r="H36">
         <f t="shared" ca="1" si="2"/>
-        <v>630</v>
+        <v>967</v>
       </c>
       <c r="I36" t="s">
         <v>134</v>
@@ -7228,19 +7228,19 @@
       </c>
       <c r="E37">
         <f t="shared" ca="1" si="2"/>
-        <v>445</v>
+        <v>836</v>
       </c>
       <c r="F37">
         <f t="shared" ca="1" si="2"/>
-        <v>272</v>
+        <v>22</v>
       </c>
       <c r="G37">
         <f t="shared" ca="1" si="2"/>
-        <v>676</v>
+        <v>747</v>
       </c>
       <c r="H37">
         <f t="shared" ca="1" si="2"/>
-        <v>211</v>
+        <v>914</v>
       </c>
       <c r="I37" t="s">
         <v>134</v>
@@ -7258,23 +7258,23 @@
       </c>
       <c r="D38">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E38">
         <f t="shared" ca="1" si="2"/>
-        <v>585</v>
+        <v>69</v>
       </c>
       <c r="F38">
         <f t="shared" ca="1" si="2"/>
-        <v>743</v>
+        <v>785</v>
       </c>
       <c r="G38">
         <f t="shared" ca="1" si="2"/>
-        <v>830</v>
+        <v>60</v>
       </c>
       <c r="H38">
         <f t="shared" ca="1" si="2"/>
-        <v>600</v>
+        <v>860</v>
       </c>
       <c r="I38" t="s">
         <v>134</v>
@@ -7292,15 +7292,15 @@
       </c>
       <c r="D39">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F39">
         <f t="shared" ca="1" si="2"/>
-        <v>771</v>
+        <v>701</v>
       </c>
       <c r="H39">
         <f t="shared" ca="1" si="2"/>
-        <v>222</v>
+        <v>625</v>
       </c>
       <c r="I39" t="s">
         <v>134</v>
@@ -7318,23 +7318,23 @@
       </c>
       <c r="D40">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E40">
         <f t="shared" ca="1" si="2"/>
-        <v>250</v>
+        <v>940</v>
       </c>
       <c r="F40">
         <f t="shared" ca="1" si="2"/>
-        <v>370</v>
+        <v>447</v>
       </c>
       <c r="G40">
         <f t="shared" ca="1" si="2"/>
-        <v>908</v>
+        <v>216</v>
       </c>
       <c r="H40">
         <f t="shared" ca="1" si="2"/>
-        <v>588</v>
+        <v>287</v>
       </c>
       <c r="I40" t="s">
         <v>133</v>
@@ -7352,23 +7352,23 @@
       </c>
       <c r="D41">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E41">
         <f t="shared" ca="1" si="2"/>
-        <v>151</v>
+        <v>650</v>
       </c>
       <c r="F41">
         <f t="shared" ca="1" si="2"/>
-        <v>917</v>
+        <v>357</v>
       </c>
       <c r="G41">
         <f t="shared" ca="1" si="2"/>
-        <v>279</v>
+        <v>213</v>
       </c>
       <c r="H41">
         <f t="shared" ca="1" si="2"/>
-        <v>893</v>
+        <v>591</v>
       </c>
       <c r="I41" t="s">
         <v>135</v>
@@ -7386,23 +7386,23 @@
       </c>
       <c r="D42">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E42">
         <f t="shared" ca="1" si="2"/>
-        <v>758</v>
+        <v>593</v>
       </c>
       <c r="F42">
         <f t="shared" ca="1" si="2"/>
-        <v>539</v>
+        <v>867</v>
       </c>
       <c r="G42">
         <f t="shared" ca="1" si="2"/>
-        <v>303</v>
+        <v>769</v>
       </c>
       <c r="H42">
         <f t="shared" ca="1" si="2"/>
-        <v>655</v>
+        <v>37</v>
       </c>
       <c r="I42" t="s">
         <v>134</v>
@@ -7420,23 +7420,23 @@
       </c>
       <c r="D43">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E43">
         <f t="shared" ca="1" si="2"/>
-        <v>611</v>
+        <v>123</v>
       </c>
       <c r="F43">
         <f t="shared" ca="1" si="2"/>
-        <v>125</v>
+        <v>298</v>
       </c>
       <c r="G43">
         <f t="shared" ca="1" si="2"/>
-        <v>565</v>
+        <v>793</v>
       </c>
       <c r="H43">
         <f t="shared" ca="1" si="2"/>
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="I43" t="s">
         <v>134</v>
@@ -7454,19 +7454,19 @@
       </c>
       <c r="E44">
         <f t="shared" ca="1" si="2"/>
-        <v>85</v>
+        <v>228</v>
       </c>
       <c r="F44">
         <f t="shared" ca="1" si="2"/>
-        <v>361</v>
+        <v>846</v>
       </c>
       <c r="G44">
         <f t="shared" ca="1" si="2"/>
-        <v>697</v>
+        <v>679</v>
       </c>
       <c r="H44">
         <f t="shared" ca="1" si="2"/>
-        <v>279</v>
+        <v>894</v>
       </c>
       <c r="I44" t="s">
         <v>134</v>
@@ -7484,23 +7484,23 @@
       </c>
       <c r="D45">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E45">
         <f t="shared" ca="1" si="2"/>
-        <v>836</v>
+        <v>653</v>
       </c>
       <c r="F45">
         <f t="shared" ca="1" si="2"/>
-        <v>107</v>
+        <v>974</v>
       </c>
       <c r="G45">
         <f t="shared" ca="1" si="2"/>
-        <v>988</v>
+        <v>127</v>
       </c>
       <c r="H45">
         <f t="shared" ca="1" si="2"/>
-        <v>299</v>
+        <v>171</v>
       </c>
       <c r="I45" t="s">
         <v>134</v>
@@ -7518,23 +7518,23 @@
       </c>
       <c r="D46">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E46">
         <f t="shared" ca="1" si="2"/>
-        <v>204</v>
+        <v>169</v>
       </c>
       <c r="F46">
         <f t="shared" ca="1" si="2"/>
-        <v>483</v>
+        <v>796</v>
       </c>
       <c r="G46">
         <f t="shared" ca="1" si="2"/>
-        <v>528</v>
+        <v>200</v>
       </c>
       <c r="H46">
         <f t="shared" ca="1" si="2"/>
-        <v>152</v>
+        <v>375</v>
       </c>
       <c r="I46" t="s">
         <v>134</v>
@@ -7556,19 +7556,19 @@
       </c>
       <c r="E47">
         <f t="shared" ca="1" si="2"/>
-        <v>733</v>
+        <v>836</v>
       </c>
       <c r="F47">
         <f t="shared" ca="1" si="2"/>
-        <v>528</v>
+        <v>150</v>
       </c>
       <c r="G47">
         <f t="shared" ca="1" si="2"/>
-        <v>347</v>
+        <v>956</v>
       </c>
       <c r="H47">
         <f t="shared" ca="1" si="2"/>
-        <v>149</v>
+        <v>735</v>
       </c>
       <c r="I47" t="s">
         <v>134</v>
@@ -7586,23 +7586,23 @@
       </c>
       <c r="D48">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E48">
         <f t="shared" ca="1" si="2"/>
-        <v>369</v>
+        <v>503</v>
       </c>
       <c r="F48">
         <f t="shared" ca="1" si="2"/>
-        <v>39</v>
+        <v>691</v>
       </c>
       <c r="G48">
         <f t="shared" ca="1" si="2"/>
-        <v>451</v>
+        <v>212</v>
       </c>
       <c r="H48">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>235</v>
       </c>
       <c r="I48" t="s">
         <v>133</v>
@@ -7620,23 +7620,23 @@
       </c>
       <c r="D49">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E49">
         <f t="shared" ca="1" si="2"/>
-        <v>872</v>
+        <v>664</v>
       </c>
       <c r="F49">
         <f t="shared" ca="1" si="2"/>
-        <v>592</v>
+        <v>453</v>
       </c>
       <c r="G49">
         <f t="shared" ca="1" si="2"/>
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="H49">
         <f t="shared" ca="1" si="2"/>
-        <v>858</v>
+        <v>593</v>
       </c>
       <c r="I49" t="s">
         <v>133</v>
@@ -7654,19 +7654,19 @@
       </c>
       <c r="D50">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E50">
         <f t="shared" ca="1" si="2"/>
-        <v>412</v>
+        <v>568</v>
       </c>
       <c r="G50">
         <f t="shared" ca="1" si="2"/>
-        <v>731</v>
+        <v>777</v>
       </c>
       <c r="H50">
         <f t="shared" ca="1" si="2"/>
-        <v>92</v>
+        <v>672</v>
       </c>
       <c r="I50" t="s">
         <v>133</v>
@@ -7684,23 +7684,23 @@
       </c>
       <c r="D51">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E51">
         <f t="shared" ca="1" si="2"/>
-        <v>522</v>
+        <v>199</v>
       </c>
       <c r="F51">
         <f t="shared" ca="1" si="2"/>
-        <v>899</v>
+        <v>340</v>
       </c>
       <c r="G51">
         <f t="shared" ca="1" si="2"/>
-        <v>791</v>
+        <v>581</v>
       </c>
       <c r="H51">
         <f t="shared" ca="1" si="2"/>
-        <v>29</v>
+        <v>285</v>
       </c>
       <c r="I51" t="s">
         <v>135</v>
@@ -7718,23 +7718,23 @@
       </c>
       <c r="D52">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E52">
         <f t="shared" ca="1" si="2"/>
-        <v>990</v>
+        <v>551</v>
       </c>
       <c r="F52">
         <f t="shared" ca="1" si="2"/>
-        <v>332</v>
+        <v>830</v>
       </c>
       <c r="G52">
         <f t="shared" ca="1" si="2"/>
-        <v>512</v>
+        <v>543</v>
       </c>
       <c r="H52">
         <f t="shared" ca="1" si="2"/>
-        <v>994</v>
+        <v>218</v>
       </c>
       <c r="I52" t="s">
         <v>134</v>
@@ -7752,23 +7752,23 @@
       </c>
       <c r="D53">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E53">
         <f t="shared" ca="1" si="2"/>
-        <v>122</v>
+        <v>89</v>
       </c>
       <c r="F53">
         <f t="shared" ca="1" si="2"/>
-        <v>849</v>
+        <v>345</v>
       </c>
       <c r="G53">
         <f t="shared" ca="1" si="2"/>
-        <v>239</v>
+        <v>464</v>
       </c>
       <c r="H53">
         <f t="shared" ca="1" si="2"/>
-        <v>427</v>
+        <v>732</v>
       </c>
       <c r="I53" t="s">
         <v>133</v>
@@ -7786,23 +7786,23 @@
       </c>
       <c r="D54">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E54">
         <f t="shared" ca="1" si="2"/>
-        <v>677</v>
+        <v>493</v>
       </c>
       <c r="F54">
         <f t="shared" ca="1" si="2"/>
-        <v>710</v>
+        <v>509</v>
       </c>
       <c r="G54">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>477</v>
       </c>
       <c r="H54">
         <f t="shared" ca="1" si="2"/>
-        <v>574</v>
+        <v>983</v>
       </c>
       <c r="I54" t="s">
         <v>133</v>
@@ -7820,19 +7820,19 @@
       </c>
       <c r="D55">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E55">
         <f t="shared" ca="1" si="2"/>
-        <v>700</v>
+        <v>406</v>
       </c>
       <c r="F55">
         <f t="shared" ca="1" si="2"/>
-        <v>187</v>
+        <v>508</v>
       </c>
       <c r="H55">
         <f t="shared" ca="1" si="2"/>
-        <v>438</v>
+        <v>618</v>
       </c>
       <c r="I55" t="s">
         <v>133</v>
@@ -7850,23 +7850,23 @@
       </c>
       <c r="D56">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E56">
         <f t="shared" ca="1" si="2"/>
-        <v>479</v>
+        <v>733</v>
       </c>
       <c r="F56">
         <f t="shared" ca="1" si="2"/>
-        <v>118</v>
+        <v>3</v>
       </c>
       <c r="G56">
         <f t="shared" ca="1" si="2"/>
-        <v>736</v>
+        <v>86</v>
       </c>
       <c r="H56">
         <f t="shared" ca="1" si="2"/>
-        <v>967</v>
+        <v>696</v>
       </c>
       <c r="I56" t="s">
         <v>134</v>
@@ -7884,23 +7884,23 @@
       </c>
       <c r="D57">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E57">
         <f t="shared" ca="1" si="2"/>
-        <v>831</v>
+        <v>198</v>
       </c>
       <c r="F57">
         <f t="shared" ca="1" si="2"/>
-        <v>810</v>
+        <v>788</v>
       </c>
       <c r="G57">
         <f t="shared" ca="1" si="2"/>
-        <v>516</v>
+        <v>53</v>
       </c>
       <c r="H57">
         <f t="shared" ca="1" si="2"/>
-        <v>745</v>
+        <v>531</v>
       </c>
       <c r="I57" t="s">
         <v>134</v>
@@ -7918,23 +7918,23 @@
       </c>
       <c r="D58">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E58">
         <f t="shared" ca="1" si="2"/>
-        <v>76</v>
+        <v>775</v>
       </c>
       <c r="F58">
         <f t="shared" ca="1" si="2"/>
-        <v>327</v>
+        <v>949</v>
       </c>
       <c r="G58">
         <f t="shared" ca="1" si="2"/>
-        <v>543</v>
+        <v>723</v>
       </c>
       <c r="H58">
         <f t="shared" ca="1" si="2"/>
-        <v>84</v>
+        <v>652</v>
       </c>
       <c r="I58" t="s">
         <v>133</v>
@@ -7952,23 +7952,23 @@
       </c>
       <c r="D59">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E59">
         <f t="shared" ca="1" si="2"/>
-        <v>135</v>
+        <v>607</v>
       </c>
       <c r="F59">
         <f t="shared" ca="1" si="2"/>
-        <v>392</v>
+        <v>105</v>
       </c>
       <c r="G59">
         <f t="shared" ca="1" si="2"/>
-        <v>198</v>
+        <v>438</v>
       </c>
       <c r="H59">
         <f t="shared" ca="1" si="2"/>
-        <v>535</v>
+        <v>313</v>
       </c>
       <c r="I59" t="s">
         <v>134</v>
@@ -7986,19 +7986,19 @@
       </c>
       <c r="D60">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E60">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>194</v>
       </c>
       <c r="G60">
         <f t="shared" ca="1" si="2"/>
-        <v>262</v>
+        <v>513</v>
       </c>
       <c r="H60">
         <f t="shared" ca="1" si="2"/>
-        <v>854</v>
+        <v>729</v>
       </c>
       <c r="I60" t="s">
         <v>135</v>
@@ -8016,23 +8016,23 @@
       </c>
       <c r="D61">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E61">
         <f t="shared" ca="1" si="2"/>
-        <v>326</v>
+        <v>155</v>
       </c>
       <c r="F61">
         <f t="shared" ca="1" si="2"/>
-        <v>195</v>
+        <v>50</v>
       </c>
       <c r="G61">
         <f t="shared" ca="1" si="2"/>
-        <v>314</v>
+        <v>631</v>
       </c>
       <c r="H61">
         <f t="shared" ca="1" si="2"/>
-        <v>187</v>
+        <v>207</v>
       </c>
       <c r="I61" t="s">
         <v>134</v>
@@ -8050,23 +8050,23 @@
       </c>
       <c r="D62">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E62">
         <f t="shared" ca="1" si="2"/>
-        <v>467</v>
+        <v>480</v>
       </c>
       <c r="F62">
         <f t="shared" ca="1" si="2"/>
-        <v>209</v>
+        <v>166</v>
       </c>
       <c r="G62">
         <f t="shared" ca="1" si="2"/>
-        <v>808</v>
+        <v>575</v>
       </c>
       <c r="H62">
         <f t="shared" ca="1" si="2"/>
-        <v>842</v>
+        <v>24</v>
       </c>
       <c r="I62" t="s">
         <v>134</v>
@@ -8084,23 +8084,23 @@
       </c>
       <c r="D63">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E63">
         <f t="shared" ca="1" si="2"/>
-        <v>905</v>
+        <v>762</v>
       </c>
       <c r="F63">
         <f t="shared" ca="1" si="2"/>
-        <v>592</v>
+        <v>490</v>
       </c>
       <c r="G63">
         <f t="shared" ca="1" si="2"/>
-        <v>760</v>
+        <v>376</v>
       </c>
       <c r="H63">
         <f t="shared" ca="1" si="2"/>
-        <v>562</v>
+        <v>315</v>
       </c>
       <c r="I63" t="s">
         <v>133</v>
@@ -8118,23 +8118,23 @@
       </c>
       <c r="D64">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E64">
         <f t="shared" ca="1" si="2"/>
-        <v>696</v>
+        <v>492</v>
       </c>
       <c r="F64">
         <f t="shared" ca="1" si="2"/>
-        <v>863</v>
+        <v>395</v>
       </c>
       <c r="G64">
         <f t="shared" ca="1" si="2"/>
-        <v>991</v>
+        <v>44</v>
       </c>
       <c r="H64">
         <f t="shared" ca="1" si="2"/>
-        <v>363</v>
+        <v>523</v>
       </c>
       <c r="I64" t="s">
         <v>134</v>
@@ -8152,23 +8152,23 @@
       </c>
       <c r="D65">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E65">
         <f t="shared" ca="1" si="2"/>
-        <v>101</v>
+        <v>582</v>
       </c>
       <c r="F65">
         <f t="shared" ca="1" si="2"/>
-        <v>574</v>
+        <v>750</v>
       </c>
       <c r="G65">
         <f t="shared" ca="1" si="2"/>
-        <v>720</v>
+        <v>54</v>
       </c>
       <c r="H65">
         <f t="shared" ca="1" si="2"/>
-        <v>560</v>
+        <v>21</v>
       </c>
       <c r="I65" t="s">
         <v>133</v>
@@ -8186,23 +8186,23 @@
       </c>
       <c r="D66">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E66">
         <f t="shared" ca="1" si="2"/>
-        <v>381</v>
+        <v>170</v>
       </c>
       <c r="F66">
         <f t="shared" ca="1" si="2"/>
-        <v>895</v>
+        <v>125</v>
       </c>
       <c r="G66">
         <f t="shared" ca="1" si="2"/>
-        <v>699</v>
+        <v>795</v>
       </c>
       <c r="H66">
         <f t="shared" ca="1" si="2"/>
-        <v>828</v>
+        <v>877</v>
       </c>
       <c r="I66" t="s">
         <v>134</v>
@@ -8220,23 +8220,23 @@
       </c>
       <c r="D67">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E67">
         <f t="shared" ca="1" si="2"/>
-        <v>553</v>
+        <v>468</v>
       </c>
       <c r="F67">
         <f t="shared" ca="1" si="2"/>
-        <v>799</v>
+        <v>10</v>
       </c>
       <c r="G67">
         <f t="shared" ca="1" si="2"/>
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="H67">
         <f t="shared" ca="1" si="2"/>
-        <v>522</v>
+        <v>691</v>
       </c>
       <c r="I67" t="s">
         <v>134</v>
@@ -8254,23 +8254,23 @@
       </c>
       <c r="D68">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E68">
         <f t="shared" ca="1" si="2"/>
-        <v>894</v>
+        <v>634</v>
       </c>
       <c r="F68">
         <f t="shared" ca="1" si="2"/>
-        <v>685</v>
+        <v>496</v>
       </c>
       <c r="G68">
         <f t="shared" ca="1" si="2"/>
-        <v>482</v>
+        <v>340</v>
       </c>
       <c r="H68">
         <f t="shared" ca="1" si="2"/>
-        <v>615</v>
+        <v>676</v>
       </c>
       <c r="I68" t="s">
         <v>134</v>
@@ -8292,19 +8292,19 @@
       </c>
       <c r="E69">
         <f t="shared" ref="E69:H97" ca="1" si="4">FLOOR(RAND()*1000,1)</f>
-        <v>827</v>
+        <v>9</v>
       </c>
       <c r="F69">
         <f t="shared" ca="1" si="4"/>
-        <v>74</v>
+        <v>396</v>
       </c>
       <c r="G69">
         <f t="shared" ca="1" si="4"/>
-        <v>917</v>
+        <v>425</v>
       </c>
       <c r="H69">
         <f t="shared" ca="1" si="4"/>
-        <v>227</v>
+        <v>285</v>
       </c>
       <c r="I69" t="s">
         <v>135</v>
@@ -8322,23 +8322,23 @@
       </c>
       <c r="D70">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E70">
         <f t="shared" ca="1" si="4"/>
-        <v>985</v>
+        <v>436</v>
       </c>
       <c r="F70">
         <f t="shared" ca="1" si="4"/>
-        <v>720</v>
+        <v>18</v>
       </c>
       <c r="G70">
         <f t="shared" ca="1" si="4"/>
-        <v>763</v>
+        <v>421</v>
       </c>
       <c r="H70">
         <f t="shared" ca="1" si="4"/>
-        <v>504</v>
+        <v>197</v>
       </c>
       <c r="I70" t="s">
         <v>134</v>
@@ -8356,23 +8356,23 @@
       </c>
       <c r="D71">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E71">
         <f t="shared" ca="1" si="4"/>
-        <v>90</v>
+        <v>347</v>
       </c>
       <c r="F71">
         <f t="shared" ca="1" si="4"/>
-        <v>205</v>
+        <v>412</v>
       </c>
       <c r="G71">
         <f t="shared" ca="1" si="4"/>
-        <v>202</v>
+        <v>386</v>
       </c>
       <c r="H71">
         <f t="shared" ca="1" si="4"/>
-        <v>821</v>
+        <v>338</v>
       </c>
       <c r="I71" t="s">
         <v>134</v>
@@ -8390,23 +8390,23 @@
       </c>
       <c r="D72">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E72">
         <f t="shared" ca="1" si="4"/>
-        <v>319</v>
+        <v>882</v>
       </c>
       <c r="F72">
         <f t="shared" ca="1" si="4"/>
-        <v>968</v>
+        <v>529</v>
       </c>
       <c r="G72">
         <f t="shared" ca="1" si="4"/>
-        <v>368</v>
+        <v>228</v>
       </c>
       <c r="H72">
         <f t="shared" ca="1" si="4"/>
-        <v>262</v>
+        <v>595</v>
       </c>
       <c r="I72" t="s">
         <v>133</v>
@@ -8424,23 +8424,23 @@
       </c>
       <c r="D73">
         <f t="shared" ca="1" si="3"/>
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E73">
         <f t="shared" ca="1" si="4"/>
-        <v>862</v>
+        <v>564</v>
       </c>
       <c r="F73">
         <f t="shared" ca="1" si="4"/>
-        <v>436</v>
+        <v>270</v>
       </c>
       <c r="G73">
         <f t="shared" ca="1" si="4"/>
-        <v>970</v>
+        <v>625</v>
       </c>
       <c r="H73">
         <f t="shared" ca="1" si="4"/>
-        <v>161</v>
+        <v>83</v>
       </c>
       <c r="I73" t="s">
         <v>133</v>
@@ -8458,23 +8458,23 @@
       </c>
       <c r="D74">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E74">
         <f t="shared" ca="1" si="4"/>
-        <v>744</v>
+        <v>498</v>
       </c>
       <c r="F74">
         <f t="shared" ca="1" si="4"/>
-        <v>308</v>
+        <v>160</v>
       </c>
       <c r="G74">
         <f t="shared" ca="1" si="4"/>
-        <v>885</v>
+        <v>545</v>
       </c>
       <c r="H74">
         <f t="shared" ca="1" si="4"/>
-        <v>266</v>
+        <v>673</v>
       </c>
       <c r="I74" t="s">
         <v>134</v>
@@ -8492,23 +8492,23 @@
       </c>
       <c r="D75">
         <f t="shared" ca="1" si="3"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E75">
         <f t="shared" ca="1" si="4"/>
-        <v>807</v>
+        <v>661</v>
       </c>
       <c r="F75">
         <f t="shared" ca="1" si="4"/>
-        <v>116</v>
+        <v>618</v>
       </c>
       <c r="G75">
         <f t="shared" ca="1" si="4"/>
-        <v>352</v>
+        <v>895</v>
       </c>
       <c r="H75">
         <f t="shared" ca="1" si="4"/>
-        <v>950</v>
+        <v>641</v>
       </c>
       <c r="I75" t="s">
         <v>134</v>
@@ -8526,23 +8526,23 @@
       </c>
       <c r="D76">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E76">
         <f t="shared" ca="1" si="4"/>
-        <v>160</v>
+        <v>22</v>
       </c>
       <c r="F76">
         <f t="shared" ca="1" si="4"/>
-        <v>834</v>
+        <v>715</v>
       </c>
       <c r="G76">
         <f t="shared" ca="1" si="4"/>
-        <v>762</v>
+        <v>806</v>
       </c>
       <c r="H76">
         <f t="shared" ca="1" si="4"/>
-        <v>382</v>
+        <v>109</v>
       </c>
       <c r="I76" t="s">
         <v>134</v>
@@ -8560,23 +8560,23 @@
       </c>
       <c r="D77">
         <f t="shared" ca="1" si="3"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E77">
         <f t="shared" ca="1" si="4"/>
-        <v>38</v>
+        <v>892</v>
       </c>
       <c r="F77">
         <f t="shared" ca="1" si="4"/>
-        <v>139</v>
+        <v>609</v>
       </c>
       <c r="G77">
         <f t="shared" ca="1" si="4"/>
-        <v>341</v>
+        <v>751</v>
       </c>
       <c r="H77">
         <f t="shared" ca="1" si="4"/>
-        <v>414</v>
+        <v>92</v>
       </c>
       <c r="I77" t="s">
         <v>135</v>
@@ -8594,23 +8594,23 @@
       </c>
       <c r="D78">
         <f t="shared" ca="1" si="3"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E78">
         <f t="shared" ca="1" si="4"/>
-        <v>342</v>
+        <v>687</v>
       </c>
       <c r="F78">
         <f t="shared" ca="1" si="4"/>
-        <v>633</v>
+        <v>721</v>
       </c>
       <c r="G78">
         <f t="shared" ca="1" si="4"/>
-        <v>762</v>
+        <v>893</v>
       </c>
       <c r="H78">
         <f t="shared" ca="1" si="4"/>
-        <v>822</v>
+        <v>317</v>
       </c>
       <c r="I78" t="s">
         <v>133</v>
@@ -8628,23 +8628,23 @@
       </c>
       <c r="D79">
         <f t="shared" ca="1" si="3"/>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E79">
         <f t="shared" ca="1" si="4"/>
-        <v>215</v>
+        <v>997</v>
       </c>
       <c r="F79">
         <f t="shared" ca="1" si="4"/>
-        <v>625</v>
+        <v>581</v>
       </c>
       <c r="G79">
         <f t="shared" ca="1" si="4"/>
-        <v>490</v>
+        <v>105</v>
       </c>
       <c r="H79">
         <f t="shared" ca="1" si="4"/>
-        <v>499</v>
+        <v>700</v>
       </c>
       <c r="I79" t="s">
         <v>134</v>
@@ -8662,23 +8662,23 @@
       </c>
       <c r="D80">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E80">
         <f t="shared" ca="1" si="4"/>
-        <v>61</v>
+        <v>685</v>
       </c>
       <c r="F80">
         <f t="shared" ca="1" si="4"/>
-        <v>428</v>
+        <v>155</v>
       </c>
       <c r="G80">
         <f t="shared" ca="1" si="4"/>
-        <v>626</v>
+        <v>962</v>
       </c>
       <c r="H80">
         <f t="shared" ca="1" si="4"/>
-        <v>247</v>
+        <v>352</v>
       </c>
       <c r="I80" t="s">
         <v>133</v>
@@ -8700,19 +8700,19 @@
       </c>
       <c r="E81">
         <f t="shared" ca="1" si="4"/>
-        <v>898</v>
+        <v>221</v>
       </c>
       <c r="F81">
         <f t="shared" ca="1" si="4"/>
-        <v>957</v>
+        <v>343</v>
       </c>
       <c r="G81">
         <f t="shared" ca="1" si="4"/>
-        <v>103</v>
+        <v>907</v>
       </c>
       <c r="H81">
         <f t="shared" ca="1" si="4"/>
-        <v>599</v>
+        <v>120</v>
       </c>
       <c r="I81" t="s">
         <v>135</v>
@@ -8734,19 +8734,19 @@
       </c>
       <c r="E82">
         <f t="shared" ca="1" si="4"/>
-        <v>919</v>
+        <v>199</v>
       </c>
       <c r="F82">
         <f t="shared" ca="1" si="4"/>
-        <v>698</v>
+        <v>245</v>
       </c>
       <c r="G82">
         <f t="shared" ca="1" si="4"/>
-        <v>515</v>
+        <v>167</v>
       </c>
       <c r="H82">
         <f t="shared" ca="1" si="4"/>
-        <v>37</v>
+        <v>371</v>
       </c>
       <c r="I82" t="s">
         <v>134</v>
@@ -8764,23 +8764,23 @@
       </c>
       <c r="D83">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E83">
         <f t="shared" ca="1" si="4"/>
-        <v>614</v>
+        <v>324</v>
       </c>
       <c r="F83">
         <f t="shared" ca="1" si="4"/>
-        <v>258</v>
+        <v>821</v>
       </c>
       <c r="G83">
         <f t="shared" ca="1" si="4"/>
-        <v>207</v>
+        <v>612</v>
       </c>
       <c r="H83">
         <f t="shared" ca="1" si="4"/>
-        <v>675</v>
+        <v>720</v>
       </c>
       <c r="I83" t="s">
         <v>135</v>
@@ -8798,23 +8798,23 @@
       </c>
       <c r="D84">
         <f t="shared" ca="1" si="3"/>
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E84">
         <f t="shared" ca="1" si="4"/>
-        <v>824</v>
+        <v>805</v>
       </c>
       <c r="F84">
         <f t="shared" ca="1" si="4"/>
-        <v>71</v>
+        <v>544</v>
       </c>
       <c r="G84">
         <f t="shared" ca="1" si="4"/>
-        <v>413</v>
+        <v>405</v>
       </c>
       <c r="H84">
         <f t="shared" ca="1" si="4"/>
-        <v>479</v>
+        <v>646</v>
       </c>
       <c r="I84" t="s">
         <v>135</v>
@@ -8832,23 +8832,23 @@
       </c>
       <c r="D85">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E85">
         <f t="shared" ca="1" si="4"/>
-        <v>214</v>
+        <v>724</v>
       </c>
       <c r="F85">
         <f t="shared" ca="1" si="4"/>
-        <v>568</v>
+        <v>352</v>
       </c>
       <c r="G85">
         <f t="shared" ca="1" si="4"/>
-        <v>260</v>
+        <v>269</v>
       </c>
       <c r="H85">
         <f t="shared" ca="1" si="4"/>
-        <v>646</v>
+        <v>317</v>
       </c>
       <c r="I85" t="s">
         <v>133</v>
@@ -8866,23 +8866,23 @@
       </c>
       <c r="D86">
         <f t="shared" ca="1" si="3"/>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E86">
         <f t="shared" ca="1" si="4"/>
-        <v>378</v>
+        <v>839</v>
       </c>
       <c r="F86">
         <f t="shared" ca="1" si="4"/>
-        <v>828</v>
+        <v>354</v>
       </c>
       <c r="G86">
         <f t="shared" ca="1" si="4"/>
-        <v>252</v>
+        <v>954</v>
       </c>
       <c r="H86">
         <f t="shared" ca="1" si="4"/>
-        <v>636</v>
+        <v>159</v>
       </c>
       <c r="I86" t="s">
         <v>134</v>
@@ -8900,23 +8900,23 @@
       </c>
       <c r="D87">
         <f t="shared" ca="1" si="3"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E87">
         <f t="shared" ca="1" si="4"/>
-        <v>83</v>
+        <v>522</v>
       </c>
       <c r="F87">
         <f t="shared" ca="1" si="4"/>
-        <v>993</v>
+        <v>485</v>
       </c>
       <c r="G87">
         <f t="shared" ca="1" si="4"/>
-        <v>755</v>
+        <v>51</v>
       </c>
       <c r="H87">
         <f t="shared" ca="1" si="4"/>
-        <v>52</v>
+        <v>197</v>
       </c>
       <c r="I87" t="s">
         <v>134</v>
@@ -8934,23 +8934,23 @@
       </c>
       <c r="D88">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E88">
         <f t="shared" ca="1" si="4"/>
-        <v>633</v>
+        <v>623</v>
       </c>
       <c r="F88">
         <f t="shared" ca="1" si="4"/>
-        <v>929</v>
+        <v>663</v>
       </c>
       <c r="G88">
         <f t="shared" ca="1" si="4"/>
-        <v>759</v>
+        <v>457</v>
       </c>
       <c r="H88">
         <f t="shared" ca="1" si="4"/>
-        <v>720</v>
+        <v>176</v>
       </c>
       <c r="I88" t="s">
         <v>133</v>
@@ -8972,19 +8972,19 @@
       </c>
       <c r="E89">
         <f t="shared" ca="1" si="4"/>
-        <v>627</v>
+        <v>888</v>
       </c>
       <c r="F89">
         <f t="shared" ca="1" si="4"/>
-        <v>903</v>
+        <v>622</v>
       </c>
       <c r="G89">
         <f t="shared" ca="1" si="4"/>
-        <v>958</v>
+        <v>73</v>
       </c>
       <c r="H89">
         <f t="shared" ca="1" si="4"/>
-        <v>758</v>
+        <v>160</v>
       </c>
       <c r="I89" t="s">
         <v>135</v>
@@ -9002,23 +9002,23 @@
       </c>
       <c r="D90">
         <f t="shared" ca="1" si="3"/>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E90">
         <f t="shared" ca="1" si="4"/>
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="F90">
         <f t="shared" ca="1" si="4"/>
-        <v>262</v>
+        <v>773</v>
       </c>
       <c r="G90">
         <f t="shared" ca="1" si="4"/>
-        <v>395</v>
+        <v>47</v>
       </c>
       <c r="H90">
         <f t="shared" ca="1" si="4"/>
-        <v>730</v>
+        <v>247</v>
       </c>
       <c r="I90" t="s">
         <v>134</v>
@@ -9036,23 +9036,23 @@
       </c>
       <c r="D91">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E91">
         <f t="shared" ca="1" si="4"/>
-        <v>190</v>
+        <v>969</v>
       </c>
       <c r="F91">
         <f t="shared" ca="1" si="4"/>
-        <v>658</v>
+        <v>241</v>
       </c>
       <c r="G91">
         <f t="shared" ca="1" si="4"/>
-        <v>690</v>
+        <v>397</v>
       </c>
       <c r="H91">
         <f t="shared" ca="1" si="4"/>
-        <v>51</v>
+        <v>430</v>
       </c>
       <c r="I91" t="s">
         <v>134</v>
@@ -9070,23 +9070,23 @@
       </c>
       <c r="D92">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E92">
         <f t="shared" ca="1" si="4"/>
-        <v>724</v>
+        <v>408</v>
       </c>
       <c r="F92">
         <f t="shared" ca="1" si="4"/>
-        <v>206</v>
+        <v>279</v>
       </c>
       <c r="G92">
         <f t="shared" ca="1" si="4"/>
-        <v>781</v>
+        <v>209</v>
       </c>
       <c r="H92">
         <f t="shared" ca="1" si="4"/>
-        <v>517</v>
+        <v>701</v>
       </c>
       <c r="I92" t="s">
         <v>133</v>
@@ -9108,19 +9108,19 @@
       </c>
       <c r="E93">
         <f t="shared" ca="1" si="4"/>
-        <v>518</v>
+        <v>631</v>
       </c>
       <c r="F93">
         <f t="shared" ca="1" si="4"/>
-        <v>547</v>
+        <v>522</v>
       </c>
       <c r="G93">
         <f t="shared" ca="1" si="4"/>
-        <v>975</v>
+        <v>632</v>
       </c>
       <c r="H93">
         <f t="shared" ca="1" si="4"/>
-        <v>888</v>
+        <v>242</v>
       </c>
       <c r="I93" t="s">
         <v>134</v>
@@ -9138,23 +9138,23 @@
       </c>
       <c r="D94">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E94">
         <f t="shared" ca="1" si="4"/>
-        <v>839</v>
+        <v>873</v>
       </c>
       <c r="F94">
         <f t="shared" ca="1" si="4"/>
-        <v>290</v>
+        <v>876</v>
       </c>
       <c r="G94">
         <f t="shared" ca="1" si="4"/>
-        <v>783</v>
+        <v>276</v>
       </c>
       <c r="H94">
         <f t="shared" ca="1" si="4"/>
-        <v>14</v>
+        <v>790</v>
       </c>
       <c r="I94" t="s">
         <v>134</v>
@@ -9172,23 +9172,23 @@
       </c>
       <c r="D95">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E95">
         <f t="shared" ca="1" si="4"/>
-        <v>6</v>
+        <v>535</v>
       </c>
       <c r="F95">
         <f t="shared" ca="1" si="4"/>
-        <v>194</v>
+        <v>501</v>
       </c>
       <c r="G95">
         <f t="shared" ca="1" si="4"/>
-        <v>492</v>
+        <v>826</v>
       </c>
       <c r="H95">
         <f t="shared" ca="1" si="4"/>
-        <v>209</v>
+        <v>537</v>
       </c>
       <c r="I95" t="s">
         <v>135</v>
@@ -9206,23 +9206,23 @@
       </c>
       <c r="D96">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E96">
         <f t="shared" ca="1" si="4"/>
-        <v>629</v>
+        <v>369</v>
       </c>
       <c r="F96">
         <f t="shared" ca="1" si="4"/>
-        <v>357</v>
+        <v>859</v>
       </c>
       <c r="G96">
         <f t="shared" ca="1" si="4"/>
-        <v>910</v>
+        <v>899</v>
       </c>
       <c r="H96">
         <f t="shared" ca="1" si="4"/>
-        <v>891</v>
+        <v>284</v>
       </c>
       <c r="I96" t="s">
         <v>135</v>
@@ -9240,23 +9240,23 @@
       </c>
       <c r="D97">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E97">
         <f t="shared" ca="1" si="4"/>
-        <v>927</v>
+        <v>249</v>
       </c>
       <c r="F97">
         <f t="shared" ca="1" si="4"/>
-        <v>641</v>
+        <v>254</v>
       </c>
       <c r="G97">
         <f t="shared" ca="1" si="4"/>
-        <v>127</v>
+        <v>88</v>
       </c>
       <c r="H97">
         <f t="shared" ca="1" si="4"/>
-        <v>42</v>
+        <v>639</v>
       </c>
       <c r="I97" t="s">
         <v>134</v>
@@ -9274,23 +9274,23 @@
       </c>
       <c r="D98">
         <f t="shared" ca="1" si="3"/>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E98">
         <f t="shared" ref="E98:H114" ca="1" si="5">FLOOR(RAND()*1000,1)</f>
-        <v>858</v>
+        <v>278</v>
       </c>
       <c r="F98">
         <f t="shared" ca="1" si="5"/>
-        <v>225</v>
+        <v>594</v>
       </c>
       <c r="G98">
         <f t="shared" ca="1" si="5"/>
-        <v>600</v>
+        <v>843</v>
       </c>
       <c r="H98">
         <f t="shared" ca="1" si="5"/>
-        <v>662</v>
+        <v>196</v>
       </c>
       <c r="I98" t="s">
         <v>133</v>
@@ -9308,23 +9308,23 @@
       </c>
       <c r="D99">
         <f t="shared" ca="1" si="3"/>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E99">
         <f t="shared" ca="1" si="5"/>
-        <v>26</v>
+        <v>228</v>
       </c>
       <c r="F99">
         <f t="shared" ca="1" si="5"/>
-        <v>951</v>
+        <v>110</v>
       </c>
       <c r="G99">
         <f t="shared" ca="1" si="5"/>
-        <v>820</v>
+        <v>171</v>
       </c>
       <c r="H99">
         <f t="shared" ca="1" si="5"/>
-        <v>949</v>
+        <v>322</v>
       </c>
       <c r="I99" t="s">
         <v>135</v>
@@ -9342,23 +9342,23 @@
       </c>
       <c r="D100">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E100">
         <f t="shared" ca="1" si="5"/>
-        <v>968</v>
+        <v>894</v>
       </c>
       <c r="F100">
         <f t="shared" ca="1" si="5"/>
-        <v>211</v>
+        <v>627</v>
       </c>
       <c r="G100">
         <f t="shared" ca="1" si="5"/>
-        <v>688</v>
+        <v>200</v>
       </c>
       <c r="H100">
         <f t="shared" ca="1" si="5"/>
-        <v>668</v>
+        <v>236</v>
       </c>
       <c r="I100" t="s">
         <v>134</v>
@@ -9376,23 +9376,23 @@
       </c>
       <c r="D101">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E101">
         <f t="shared" ca="1" si="5"/>
-        <v>658</v>
+        <v>48</v>
       </c>
       <c r="F101">
         <f t="shared" ca="1" si="5"/>
-        <v>81</v>
+        <v>628</v>
       </c>
       <c r="G101">
         <f t="shared" ca="1" si="5"/>
-        <v>310</v>
+        <v>122</v>
       </c>
       <c r="H101">
         <f t="shared" ca="1" si="5"/>
-        <v>4</v>
+        <v>742</v>
       </c>
       <c r="I101" t="s">
         <v>135</v>
@@ -9410,23 +9410,23 @@
       </c>
       <c r="D102">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E102">
         <f t="shared" ca="1" si="5"/>
-        <v>802</v>
+        <v>250</v>
       </c>
       <c r="F102">
         <f t="shared" ca="1" si="5"/>
-        <v>516</v>
+        <v>156</v>
       </c>
       <c r="G102">
         <f t="shared" ca="1" si="5"/>
-        <v>591</v>
+        <v>459</v>
       </c>
       <c r="H102">
         <f t="shared" ca="1" si="5"/>
-        <v>222</v>
+        <v>341</v>
       </c>
       <c r="I102" t="s">
         <v>135</v>
@@ -9444,23 +9444,23 @@
       </c>
       <c r="D103">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E103">
         <f t="shared" ca="1" si="5"/>
-        <v>18</v>
+        <v>734</v>
       </c>
       <c r="F103">
         <f t="shared" ca="1" si="5"/>
-        <v>615</v>
+        <v>624</v>
       </c>
       <c r="G103">
         <f t="shared" ca="1" si="5"/>
-        <v>32</v>
+        <v>142</v>
       </c>
       <c r="H103">
         <f t="shared" ca="1" si="5"/>
-        <v>762</v>
+        <v>499</v>
       </c>
       <c r="I103" t="s">
         <v>133</v>
@@ -9478,23 +9478,23 @@
       </c>
       <c r="D104">
         <f t="shared" ca="1" si="3"/>
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E104">
         <f t="shared" ca="1" si="5"/>
-        <v>733</v>
+        <v>867</v>
       </c>
       <c r="F104">
         <f t="shared" ca="1" si="5"/>
-        <v>692</v>
+        <v>247</v>
       </c>
       <c r="G104">
         <f t="shared" ca="1" si="5"/>
-        <v>939</v>
+        <v>715</v>
       </c>
       <c r="H104">
         <f t="shared" ca="1" si="5"/>
-        <v>522</v>
+        <v>448</v>
       </c>
       <c r="I104" t="s">
         <v>134</v>
@@ -9512,23 +9512,23 @@
       </c>
       <c r="D105">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E105">
         <f t="shared" ca="1" si="5"/>
-        <v>629</v>
+        <v>847</v>
       </c>
       <c r="F105">
         <f t="shared" ca="1" si="5"/>
-        <v>566</v>
+        <v>909</v>
       </c>
       <c r="G105">
         <f t="shared" ca="1" si="5"/>
-        <v>55</v>
+        <v>209</v>
       </c>
       <c r="H105">
         <f t="shared" ca="1" si="5"/>
-        <v>437</v>
+        <v>652</v>
       </c>
       <c r="I105" t="s">
         <v>134</v>
@@ -9546,23 +9546,23 @@
       </c>
       <c r="D106">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E106">
         <f t="shared" ca="1" si="5"/>
-        <v>359</v>
+        <v>739</v>
       </c>
       <c r="F106">
         <f t="shared" ca="1" si="5"/>
-        <v>587</v>
+        <v>601</v>
       </c>
       <c r="G106">
         <f t="shared" ca="1" si="5"/>
-        <v>226</v>
+        <v>210</v>
       </c>
       <c r="H106">
         <f t="shared" ca="1" si="5"/>
-        <v>907</v>
+        <v>701</v>
       </c>
       <c r="I106" t="s">
         <v>133</v>
@@ -9584,19 +9584,19 @@
       </c>
       <c r="E107">
         <f t="shared" ca="1" si="5"/>
-        <v>502</v>
+        <v>420</v>
       </c>
       <c r="F107">
         <f t="shared" ca="1" si="5"/>
-        <v>94</v>
+        <v>703</v>
       </c>
       <c r="G107">
         <f t="shared" ca="1" si="5"/>
-        <v>642</v>
+        <v>798</v>
       </c>
       <c r="H107">
         <f t="shared" ca="1" si="5"/>
-        <v>374</v>
+        <v>1</v>
       </c>
       <c r="I107" t="s">
         <v>135</v>
@@ -9614,23 +9614,23 @@
       </c>
       <c r="D108">
         <f t="shared" ca="1" si="3"/>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E108">
         <f t="shared" ca="1" si="5"/>
-        <v>436</v>
+        <v>330</v>
       </c>
       <c r="F108">
         <f t="shared" ca="1" si="5"/>
-        <v>314</v>
+        <v>583</v>
       </c>
       <c r="G108">
         <f t="shared" ca="1" si="5"/>
-        <v>100</v>
+        <v>662</v>
       </c>
       <c r="H108">
         <f t="shared" ca="1" si="5"/>
-        <v>106</v>
+        <v>963</v>
       </c>
       <c r="I108" t="s">
         <v>134</v>
@@ -9648,23 +9648,23 @@
       </c>
       <c r="D109">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E109">
         <f t="shared" ca="1" si="5"/>
-        <v>217</v>
+        <v>120</v>
       </c>
       <c r="F109">
         <f t="shared" ca="1" si="5"/>
-        <v>345</v>
+        <v>533</v>
       </c>
       <c r="G109">
         <f t="shared" ca="1" si="5"/>
-        <v>9</v>
+        <v>99</v>
       </c>
       <c r="H109">
         <f t="shared" ca="1" si="5"/>
-        <v>182</v>
+        <v>449</v>
       </c>
       <c r="I109" t="s">
         <v>134</v>
@@ -9682,23 +9682,23 @@
       </c>
       <c r="D110">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E110">
         <f t="shared" ca="1" si="5"/>
-        <v>552</v>
+        <v>531</v>
       </c>
       <c r="F110">
         <f t="shared" ca="1" si="5"/>
-        <v>485</v>
+        <v>198</v>
       </c>
       <c r="G110">
         <f t="shared" ca="1" si="5"/>
-        <v>712</v>
+        <v>965</v>
       </c>
       <c r="H110">
         <f t="shared" ca="1" si="5"/>
-        <v>674</v>
+        <v>162</v>
       </c>
       <c r="I110" t="s">
         <v>133</v>
@@ -9716,23 +9716,23 @@
       </c>
       <c r="D111">
         <f t="shared" ca="1" si="3"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E111">
         <f t="shared" ca="1" si="5"/>
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F111">
         <f t="shared" ca="1" si="5"/>
-        <v>376</v>
+        <v>411</v>
       </c>
       <c r="G111">
         <f t="shared" ca="1" si="5"/>
-        <v>793</v>
+        <v>229</v>
       </c>
       <c r="H111">
         <f t="shared" ca="1" si="5"/>
-        <v>328</v>
+        <v>106</v>
       </c>
       <c r="I111" t="s">
         <v>134</v>
@@ -9750,23 +9750,23 @@
       </c>
       <c r="D112">
         <f t="shared" ca="1" si="3"/>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E112">
         <f t="shared" ca="1" si="5"/>
-        <v>106</v>
+        <v>55</v>
       </c>
       <c r="F112">
         <f t="shared" ca="1" si="5"/>
-        <v>69</v>
+        <v>478</v>
       </c>
       <c r="G112">
         <f t="shared" ca="1" si="5"/>
-        <v>268</v>
+        <v>190</v>
       </c>
       <c r="H112">
         <f t="shared" ca="1" si="5"/>
-        <v>212</v>
+        <v>823</v>
       </c>
       <c r="I112" t="s">
         <v>134</v>
@@ -9788,19 +9788,19 @@
       </c>
       <c r="E113">
         <f t="shared" ca="1" si="5"/>
-        <v>492</v>
+        <v>288</v>
       </c>
       <c r="F113">
         <f t="shared" ca="1" si="5"/>
-        <v>709</v>
+        <v>503</v>
       </c>
       <c r="G113">
         <f t="shared" ca="1" si="5"/>
-        <v>439</v>
+        <v>224</v>
       </c>
       <c r="H113">
         <f t="shared" ca="1" si="5"/>
-        <v>965</v>
+        <v>532</v>
       </c>
       <c r="I113" t="s">
         <v>135</v>
@@ -9818,23 +9818,23 @@
       </c>
       <c r="D114">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E114">
         <f t="shared" ca="1" si="5"/>
-        <v>147</v>
+        <v>469</v>
       </c>
       <c r="F114">
         <f t="shared" ca="1" si="5"/>
-        <v>27</v>
+        <v>221</v>
       </c>
       <c r="G114">
         <f t="shared" ca="1" si="5"/>
-        <v>552</v>
+        <v>287</v>
       </c>
       <c r="H114">
         <f t="shared" ca="1" si="5"/>
-        <v>179</v>
+        <v>355</v>
       </c>
       <c r="I114" t="s">
         <v>135</v>
@@ -9918,7 +9918,7 @@
       </c>
       <c r="J4">
         <f ca="1">RAND()</f>
-        <v>0.24804043821990973</v>
+        <v>1.9806289990273118E-2</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
@@ -9949,7 +9949,7 @@
       </c>
       <c r="J5">
         <f t="shared" ref="J5:J68" ca="1" si="1">RAND()</f>
-        <v>0.1533723219687767</v>
+        <v>0.28076314453588525</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
@@ -9976,11 +9976,11 @@
       </c>
       <c r="I6" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>B</v>
+        <v>A</v>
       </c>
       <c r="J6">
         <f t="shared" ca="1" si="1"/>
-        <v>0.47586148360940517</v>
+        <v>0.98727763043870354</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
@@ -10011,7 +10011,7 @@
       </c>
       <c r="J7">
         <f t="shared" ca="1" si="1"/>
-        <v>0.35064919674868045</v>
+        <v>0.34979337543948497</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
@@ -10042,7 +10042,7 @@
       </c>
       <c r="J8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.6783023940833508</v>
+        <v>0.37553090900066188</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
@@ -10073,7 +10073,7 @@
       </c>
       <c r="J9">
         <f t="shared" ca="1" si="1"/>
-        <v>0.62654510169365518</v>
+        <v>0.60867747455423504</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
@@ -10100,11 +10100,11 @@
       </c>
       <c r="I10" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>C</v>
+        <v>B</v>
       </c>
       <c r="J10">
         <f t="shared" ca="1" si="1"/>
-        <v>0.12542662864805509</v>
+        <v>0.58737373069049392</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
@@ -10135,7 +10135,7 @@
       </c>
       <c r="J11">
         <f t="shared" ca="1" si="1"/>
-        <v>0.62993298761837047</v>
+        <v>0.37593936058970367</v>
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
@@ -10162,11 +10162,11 @@
       </c>
       <c r="I12" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>C</v>
+        <v>B</v>
       </c>
       <c r="J12">
         <f t="shared" ca="1" si="1"/>
-        <v>0.13880700600599016</v>
+        <v>0.57746051694175637</v>
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
@@ -10197,7 +10197,7 @@
       </c>
       <c r="J13">
         <f t="shared" ca="1" si="1"/>
-        <v>0.43433814194442644</v>
+        <v>0.65071514407089837</v>
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
@@ -10228,7 +10228,7 @@
       </c>
       <c r="J14">
         <f t="shared" ca="1" si="1"/>
-        <v>0.41828049161625369</v>
+        <v>0.49601556711014982</v>
       </c>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
@@ -10259,7 +10259,7 @@
       </c>
       <c r="J15">
         <f t="shared" ca="1" si="1"/>
-        <v>0.28037671598372726</v>
+        <v>1.3142841535917382E-2</v>
       </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
@@ -10287,7 +10287,7 @@
       </c>
       <c r="J16">
         <f t="shared" ca="1" si="1"/>
-        <v>0.31264206294381092</v>
+        <v>0.30757610662449908</v>
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
@@ -10318,7 +10318,7 @@
       </c>
       <c r="J17">
         <f t="shared" ca="1" si="1"/>
-        <v>0.26128041247561284</v>
+        <v>0.22998404566163733</v>
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
@@ -10345,11 +10345,11 @@
       </c>
       <c r="I18" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>B</v>
+        <v>C</v>
       </c>
       <c r="J18">
         <f t="shared" ca="1" si="1"/>
-        <v>0.74664137178523582</v>
+        <v>0.29810157279657401</v>
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
@@ -10380,7 +10380,7 @@
       </c>
       <c r="J19">
         <f t="shared" ca="1" si="1"/>
-        <v>0.15815034989672072</v>
+        <v>0.15068342103830545</v>
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
@@ -10407,11 +10407,11 @@
       </c>
       <c r="I20" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>B</v>
+        <v>A</v>
       </c>
       <c r="J20">
         <f t="shared" ca="1" si="1"/>
-        <v>0.65952176560913844</v>
+        <v>0.88817186782227109</v>
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
@@ -10438,11 +10438,11 @@
       </c>
       <c r="I21" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>B</v>
+        <v>A</v>
       </c>
       <c r="J21">
         <f t="shared" ca="1" si="1"/>
-        <v>0.43780709280020091</v>
+        <v>0.96163318395337105</v>
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
@@ -10473,7 +10473,7 @@
       </c>
       <c r="J22">
         <f t="shared" ca="1" si="1"/>
-        <v>0.78429657269656061</v>
+        <v>0.59103021227792785</v>
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
@@ -10504,7 +10504,7 @@
       </c>
       <c r="J23">
         <f t="shared" ca="1" si="1"/>
-        <v>0.10746287349752315</v>
+        <v>3.5095478049029571E-2</v>
       </c>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
@@ -10535,7 +10535,7 @@
       </c>
       <c r="J24">
         <f t="shared" ca="1" si="1"/>
-        <v>0.16758401461101369</v>
+        <v>0.23382650318055809</v>
       </c>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
@@ -10566,7 +10566,7 @@
       </c>
       <c r="J25">
         <f t="shared" ca="1" si="1"/>
-        <v>0.53488145647882479</v>
+        <v>0.36084087832018352</v>
       </c>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25">
@@ -10597,7 +10597,7 @@
       </c>
       <c r="J26">
         <f t="shared" ca="1" si="1"/>
-        <v>0.62757431272631026</v>
+        <v>0.47020544526783303</v>
       </c>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.25">
@@ -10624,11 +10624,11 @@
       </c>
       <c r="I27" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>B</v>
+        <v>A</v>
       </c>
       <c r="J27">
         <f t="shared" ca="1" si="1"/>
-        <v>0.72698603570466958</v>
+        <v>0.8620097388050183</v>
       </c>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.25">
@@ -10655,11 +10655,11 @@
       </c>
       <c r="I28" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>A</v>
+        <v>B</v>
       </c>
       <c r="J28">
         <f t="shared" ca="1" si="1"/>
-        <v>0.84238857406534595</v>
+        <v>0.59097277419139027</v>
       </c>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
@@ -10687,7 +10687,7 @@
       </c>
       <c r="J29">
         <f t="shared" ca="1" si="1"/>
-        <v>0.89639695456638369</v>
+        <v>0.8485072035749921</v>
       </c>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.25">
@@ -10714,11 +10714,11 @@
       </c>
       <c r="I30" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>A</v>
+        <v>B</v>
       </c>
       <c r="J30">
         <f t="shared" ca="1" si="1"/>
-        <v>0.830330307210292</v>
+        <v>0.43760136584132425</v>
       </c>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.25">
@@ -10749,7 +10749,7 @@
       </c>
       <c r="J31">
         <f t="shared" ca="1" si="1"/>
-        <v>0.70510881528935399</v>
+        <v>0.76450061565243799</v>
       </c>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.25">
@@ -10776,11 +10776,11 @@
       </c>
       <c r="I32" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>B</v>
+        <v>C</v>
       </c>
       <c r="J32">
         <f t="shared" ca="1" si="1"/>
-        <v>0.50330777458796772</v>
+        <v>6.7548833070544712E-2</v>
       </c>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.25">
@@ -10807,11 +10807,11 @@
       </c>
       <c r="I33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>A</v>
+        <v>C</v>
       </c>
       <c r="J33">
         <f t="shared" ca="1" si="1"/>
-        <v>0.8522683565544088</v>
+        <v>0.12436839462335014</v>
       </c>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.25">
@@ -10838,11 +10838,11 @@
       </c>
       <c r="I34" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>C</v>
+        <v>A</v>
       </c>
       <c r="J34">
         <f t="shared" ca="1" si="1"/>
-        <v>0.15122358002333214</v>
+        <v>0.93253040664212439</v>
       </c>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.25">
@@ -10869,11 +10869,11 @@
       </c>
       <c r="I35" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>B</v>
+        <v>C</v>
       </c>
       <c r="J35">
         <f t="shared" ca="1" si="1"/>
-        <v>0.46242442666636641</v>
+        <v>0.13100509509317348</v>
       </c>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.25">
@@ -10904,7 +10904,7 @@
       </c>
       <c r="J36">
         <f t="shared" ca="1" si="1"/>
-        <v>0.49621714035342079</v>
+        <v>0.43602916194760799</v>
       </c>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.25">
@@ -10931,11 +10931,11 @@
       </c>
       <c r="I37" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>A</v>
+        <v>B</v>
       </c>
       <c r="J37">
         <f t="shared" ca="1" si="1"/>
-        <v>0.82692685983323067</v>
+        <v>0.47033812281632004</v>
       </c>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.25">
@@ -10962,11 +10962,11 @@
       </c>
       <c r="I38" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>C</v>
+        <v>B</v>
       </c>
       <c r="J38">
         <f t="shared" ca="1" si="1"/>
-        <v>0.28019900840649758</v>
+        <v>0.32059604641894013</v>
       </c>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.25">
@@ -10987,11 +10987,11 @@
       </c>
       <c r="I39" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>A</v>
+        <v>B</v>
       </c>
       <c r="J39">
         <f t="shared" ca="1" si="1"/>
-        <v>0.88083576597649094</v>
+        <v>0.52372636653569049</v>
       </c>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.25">
@@ -11018,11 +11018,11 @@
       </c>
       <c r="I40" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>C</v>
+        <v>B</v>
       </c>
       <c r="J40">
         <f t="shared" ca="1" si="1"/>
-        <v>0.17080911170405721</v>
+        <v>0.606422912657966</v>
       </c>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.25">
@@ -11053,7 +11053,7 @@
       </c>
       <c r="J41">
         <f t="shared" ca="1" si="1"/>
-        <v>0.51694666533679279</v>
+        <v>0.34848797982133772</v>
       </c>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.25">
@@ -11080,11 +11080,11 @@
       </c>
       <c r="I42" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>C</v>
+        <v>B</v>
       </c>
       <c r="J42">
         <f t="shared" ca="1" si="1"/>
-        <v>0.12211314453605127</v>
+        <v>0.57504085793295623</v>
       </c>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.25">
@@ -11115,7 +11115,7 @@
       </c>
       <c r="J43">
         <f t="shared" ca="1" si="1"/>
-        <v>0.66605455746327424</v>
+        <v>0.52842271901479287</v>
       </c>
     </row>
     <row r="44" spans="2:10" x14ac:dyDescent="0.25">
@@ -11139,11 +11139,11 @@
       </c>
       <c r="I44" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>B</v>
+        <v>A</v>
       </c>
       <c r="J44">
         <f t="shared" ca="1" si="1"/>
-        <v>0.53311930173479583</v>
+        <v>0.87959703534147704</v>
       </c>
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.25">
@@ -11170,11 +11170,11 @@
       </c>
       <c r="I45" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>A</v>
+        <v>C</v>
       </c>
       <c r="J45">
         <f t="shared" ca="1" si="1"/>
-        <v>0.86041719945057926</v>
+        <v>0.15355718316152578</v>
       </c>
     </row>
     <row r="46" spans="2:10" x14ac:dyDescent="0.25">
@@ -11201,11 +11201,11 @@
       </c>
       <c r="I46" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>B</v>
+        <v>C</v>
       </c>
       <c r="J46">
         <f t="shared" ca="1" si="1"/>
-        <v>0.52760849068266391</v>
+        <v>0.2321634185011805</v>
       </c>
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.25">
@@ -11236,7 +11236,7 @@
       </c>
       <c r="J47">
         <f t="shared" ca="1" si="1"/>
-        <v>0.8660307805991464</v>
+        <v>0.87619578966225886</v>
       </c>
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.25">
@@ -11263,11 +11263,11 @@
       </c>
       <c r="I48" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>B</v>
+        <v>C</v>
       </c>
       <c r="J48">
         <f t="shared" ca="1" si="1"/>
-        <v>0.40878067311961086</v>
+        <v>0.14703577357783193</v>
       </c>
     </row>
     <row r="49" spans="2:10" x14ac:dyDescent="0.25">
@@ -11294,11 +11294,11 @@
       </c>
       <c r="I49" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>C</v>
+        <v>A</v>
       </c>
       <c r="J49">
         <f t="shared" ca="1" si="1"/>
-        <v>0.11594751242271295</v>
+        <v>0.80130651337120973</v>
       </c>
     </row>
     <row r="50" spans="2:10" x14ac:dyDescent="0.25">
@@ -11326,7 +11326,7 @@
       </c>
       <c r="J50">
         <f t="shared" ca="1" si="1"/>
-        <v>0.15701127490172628</v>
+        <v>1.4612159006761938E-2</v>
       </c>
     </row>
     <row r="51" spans="2:10" x14ac:dyDescent="0.25">
@@ -11353,11 +11353,11 @@
       </c>
       <c r="I51" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>B</v>
+        <v>C</v>
       </c>
       <c r="J51">
         <f t="shared" ca="1" si="1"/>
-        <v>0.55753607745967715</v>
+        <v>0.297595833450224</v>
       </c>
     </row>
     <row r="52" spans="2:10" x14ac:dyDescent="0.25">
@@ -11384,11 +11384,11 @@
       </c>
       <c r="I52" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>B</v>
+        <v>C</v>
       </c>
       <c r="J52">
         <f t="shared" ca="1" si="1"/>
-        <v>0.50221782802025117</v>
+        <v>4.1340501730540269E-2</v>
       </c>
     </row>
     <row r="53" spans="2:10" x14ac:dyDescent="0.25">
@@ -11415,11 +11415,11 @@
       </c>
       <c r="I53" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>B</v>
+        <v>A</v>
       </c>
       <c r="J53">
         <f t="shared" ca="1" si="1"/>
-        <v>0.47213255864327941</v>
+        <v>0.81224790785879142</v>
       </c>
     </row>
     <row r="54" spans="2:10" x14ac:dyDescent="0.25">
@@ -11446,11 +11446,11 @@
       </c>
       <c r="I54" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>C</v>
+        <v>B</v>
       </c>
       <c r="J54">
         <f t="shared" ca="1" si="1"/>
-        <v>0.15619172061629905</v>
+        <v>0.46787229516501272</v>
       </c>
     </row>
     <row r="55" spans="2:10" x14ac:dyDescent="0.25">
@@ -11474,11 +11474,11 @@
       </c>
       <c r="I55" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>B</v>
+        <v>C</v>
       </c>
       <c r="J55">
         <f t="shared" ca="1" si="1"/>
-        <v>0.59897473117618438</v>
+        <v>3.9654334412815739E-2</v>
       </c>
     </row>
     <row r="56" spans="2:10" x14ac:dyDescent="0.25">
@@ -11505,11 +11505,11 @@
       </c>
       <c r="I56" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>B</v>
+        <v>C</v>
       </c>
       <c r="J56">
         <f t="shared" ca="1" si="1"/>
-        <v>0.54324135967386855</v>
+        <v>5.6265261633818398E-2</v>
       </c>
     </row>
     <row r="57" spans="2:10" x14ac:dyDescent="0.25">
@@ -11536,11 +11536,11 @@
       </c>
       <c r="I57" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>C</v>
+        <v>B</v>
       </c>
       <c r="J57">
         <f t="shared" ca="1" si="1"/>
-        <v>0.19126669942974084</v>
+        <v>0.77909863488464659</v>
       </c>
     </row>
     <row r="58" spans="2:10" x14ac:dyDescent="0.25">
@@ -11571,7 +11571,7 @@
       </c>
       <c r="J58">
         <f t="shared" ca="1" si="1"/>
-        <v>0.37107774851092357</v>
+        <v>0.64550317014419556</v>
       </c>
     </row>
     <row r="59" spans="2:10" x14ac:dyDescent="0.25">
@@ -11598,11 +11598,11 @@
       </c>
       <c r="I59" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>A</v>
+        <v>C</v>
       </c>
       <c r="J59">
         <f t="shared" ca="1" si="1"/>
-        <v>0.95909479694266608</v>
+        <v>0.13777425476438765</v>
       </c>
     </row>
     <row r="60" spans="2:10" x14ac:dyDescent="0.25">
@@ -11626,11 +11626,11 @@
       </c>
       <c r="I60" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>C</v>
+        <v>A</v>
       </c>
       <c r="J60">
         <f t="shared" ca="1" si="1"/>
-        <v>0.24762427131403231</v>
+        <v>0.94550128360172059</v>
       </c>
     </row>
     <row r="61" spans="2:10" x14ac:dyDescent="0.25">
@@ -11657,11 +11657,11 @@
       </c>
       <c r="I61" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>B</v>
+        <v>C</v>
       </c>
       <c r="J61">
         <f t="shared" ca="1" si="1"/>
-        <v>0.68559998863669003</v>
+        <v>4.1225696867091655E-2</v>
       </c>
     </row>
     <row r="62" spans="2:10" x14ac:dyDescent="0.25">
@@ -11688,11 +11688,11 @@
       </c>
       <c r="I62" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>B</v>
+        <v>A</v>
       </c>
       <c r="J62">
         <f t="shared" ca="1" si="1"/>
-        <v>0.4519494287731195</v>
+        <v>0.92256298185314611</v>
       </c>
     </row>
     <row r="63" spans="2:10" x14ac:dyDescent="0.25">
@@ -11723,7 +11723,7 @@
       </c>
       <c r="J63">
         <f t="shared" ca="1" si="1"/>
-        <v>0.42362988342690322</v>
+        <v>0.55125748074610437</v>
       </c>
     </row>
     <row r="64" spans="2:10" x14ac:dyDescent="0.25">
@@ -11750,11 +11750,11 @@
       </c>
       <c r="I64" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>C</v>
+        <v>A</v>
       </c>
       <c r="J64">
         <f t="shared" ca="1" si="1"/>
-        <v>8.583499127519767E-2</v>
+        <v>0.88203685083039529</v>
       </c>
     </row>
     <row r="65" spans="2:10" x14ac:dyDescent="0.25">
@@ -11785,7 +11785,7 @@
       </c>
       <c r="J65">
         <f t="shared" ca="1" si="1"/>
-        <v>0.15659419067437819</v>
+        <v>0.22272462837283669</v>
       </c>
     </row>
     <row r="66" spans="2:10" x14ac:dyDescent="0.25">
@@ -11816,7 +11816,7 @@
       </c>
       <c r="J66">
         <f t="shared" ca="1" si="1"/>
-        <v>0.62556418097619426</v>
+        <v>0.32963702900304936</v>
       </c>
     </row>
     <row r="67" spans="2:10" x14ac:dyDescent="0.25">
@@ -11847,7 +11847,7 @@
       </c>
       <c r="J67">
         <f t="shared" ca="1" si="1"/>
-        <v>0.27202584464575563</v>
+        <v>0.10423354358261838</v>
       </c>
     </row>
     <row r="68" spans="2:10" x14ac:dyDescent="0.25">
@@ -11874,11 +11874,11 @@
       </c>
       <c r="I68" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>B</v>
+        <v>C</v>
       </c>
       <c r="J68">
         <f t="shared" ca="1" si="1"/>
-        <v>0.70452348447150803</v>
+        <v>0.11147005779757513</v>
       </c>
     </row>
     <row r="69" spans="2:10" x14ac:dyDescent="0.25">
@@ -11909,7 +11909,7 @@
       </c>
       <c r="J69">
         <f t="shared" ref="J69:J114" ca="1" si="3">RAND()</f>
-        <v>0.43832766480840901</v>
+        <v>0.37883151352989863</v>
       </c>
     </row>
     <row r="70" spans="2:10" x14ac:dyDescent="0.25">
@@ -11940,7 +11940,7 @@
       </c>
       <c r="J70">
         <f t="shared" ca="1" si="3"/>
-        <v>0.87123300316136376</v>
+        <v>0.96966192422939057</v>
       </c>
     </row>
     <row r="71" spans="2:10" x14ac:dyDescent="0.25">
@@ -11967,11 +11967,11 @@
       </c>
       <c r="I71" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>C</v>
+        <v>B</v>
       </c>
       <c r="J71">
         <f t="shared" ca="1" si="3"/>
-        <v>3.3859161324033549E-2</v>
+        <v>0.58536691930645712</v>
       </c>
     </row>
     <row r="72" spans="2:10" x14ac:dyDescent="0.25">
@@ -12002,7 +12002,7 @@
       </c>
       <c r="J72">
         <f t="shared" ca="1" si="3"/>
-        <v>0.67674122116304747</v>
+        <v>0.60355658810272317</v>
       </c>
     </row>
     <row r="73" spans="2:10" x14ac:dyDescent="0.25">
@@ -12029,11 +12029,11 @@
       </c>
       <c r="I73" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>C</v>
+        <v>B</v>
       </c>
       <c r="J73">
         <f t="shared" ca="1" si="3"/>
-        <v>0.1519674884664477</v>
+        <v>0.47056156454601095</v>
       </c>
     </row>
     <row r="74" spans="2:10" x14ac:dyDescent="0.25">
@@ -12064,7 +12064,7 @@
       </c>
       <c r="J74">
         <f t="shared" ca="1" si="3"/>
-        <v>0.44024864790871487</v>
+        <v>0.5151600279501366</v>
       </c>
     </row>
     <row r="75" spans="2:10" x14ac:dyDescent="0.25">
@@ -12091,11 +12091,11 @@
       </c>
       <c r="I75" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>A</v>
+        <v>B</v>
       </c>
       <c r="J75">
         <f t="shared" ca="1" si="3"/>
-        <v>0.84176355298460981</v>
+        <v>0.48418321647449558</v>
       </c>
     </row>
     <row r="76" spans="2:10" x14ac:dyDescent="0.25">
@@ -12126,7 +12126,7 @@
       </c>
       <c r="J76">
         <f t="shared" ca="1" si="3"/>
-        <v>0.1220516227136289</v>
+        <v>0.16800688180315915</v>
       </c>
     </row>
     <row r="77" spans="2:10" x14ac:dyDescent="0.25">
@@ -12157,7 +12157,7 @@
       </c>
       <c r="J77">
         <f t="shared" ca="1" si="3"/>
-        <v>0.16765038390052445</v>
+        <v>0.12228008201035157</v>
       </c>
     </row>
     <row r="78" spans="2:10" x14ac:dyDescent="0.25">
@@ -12184,11 +12184,11 @@
       </c>
       <c r="I78" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>C</v>
+        <v>B</v>
       </c>
       <c r="J78">
         <f t="shared" ca="1" si="3"/>
-        <v>0.14585589018784773</v>
+        <v>0.53183891118284887</v>
       </c>
     </row>
     <row r="79" spans="2:10" x14ac:dyDescent="0.25">
@@ -12219,7 +12219,7 @@
       </c>
       <c r="J79">
         <f t="shared" ca="1" si="3"/>
-        <v>0.66462100609268426</v>
+        <v>0.48192396668336046</v>
       </c>
     </row>
     <row r="80" spans="2:10" x14ac:dyDescent="0.25">
@@ -12250,7 +12250,7 @@
       </c>
       <c r="J80">
         <f t="shared" ca="1" si="3"/>
-        <v>0.93870234989254908</v>
+        <v>0.96911729709264882</v>
       </c>
     </row>
     <row r="81" spans="2:10" x14ac:dyDescent="0.25">
@@ -12281,7 +12281,7 @@
       </c>
       <c r="J81">
         <f t="shared" ca="1" si="3"/>
-        <v>0.3544194182315773</v>
+        <v>0.40983599069631516</v>
       </c>
     </row>
     <row r="82" spans="2:10" x14ac:dyDescent="0.25">
@@ -12312,7 +12312,7 @@
       </c>
       <c r="J82">
         <f t="shared" ca="1" si="3"/>
-        <v>0.25689452520691669</v>
+        <v>0.21897588199613305</v>
       </c>
     </row>
     <row r="83" spans="2:10" x14ac:dyDescent="0.25">
@@ -12343,7 +12343,7 @@
       </c>
       <c r="J83">
         <f t="shared" ca="1" si="3"/>
-        <v>0.37065390713049118</v>
+        <v>0.70296240434086743</v>
       </c>
     </row>
     <row r="84" spans="2:10" x14ac:dyDescent="0.25">
@@ -12370,11 +12370,11 @@
       </c>
       <c r="I84" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>B</v>
+        <v>C</v>
       </c>
       <c r="J84">
         <f t="shared" ca="1" si="3"/>
-        <v>0.65834343444023069</v>
+        <v>0.24054412186991148</v>
       </c>
     </row>
     <row r="85" spans="2:10" x14ac:dyDescent="0.25">
@@ -12405,7 +12405,7 @@
       </c>
       <c r="J85">
         <f t="shared" ca="1" si="3"/>
-        <v>0.47773936939262351</v>
+        <v>0.36113627370800239</v>
       </c>
     </row>
     <row r="86" spans="2:10" x14ac:dyDescent="0.25">
@@ -12436,7 +12436,7 @@
       </c>
       <c r="J86">
         <f t="shared" ca="1" si="3"/>
-        <v>0.71072564777797953</v>
+        <v>0.50024184527199933</v>
       </c>
     </row>
     <row r="87" spans="2:10" x14ac:dyDescent="0.25">
@@ -12463,11 +12463,11 @@
       </c>
       <c r="I87" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>B</v>
+        <v>A</v>
       </c>
       <c r="J87">
         <f t="shared" ca="1" si="3"/>
-        <v>0.65269985099794359</v>
+        <v>0.9007921946234817</v>
       </c>
     </row>
     <row r="88" spans="2:10" x14ac:dyDescent="0.25">
@@ -12494,11 +12494,11 @@
       </c>
       <c r="I88" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>C</v>
+        <v>B</v>
       </c>
       <c r="J88">
         <f t="shared" ca="1" si="3"/>
-        <v>0.20269684822940981</v>
+        <v>0.31259230588760956</v>
       </c>
     </row>
     <row r="89" spans="2:10" x14ac:dyDescent="0.25">
@@ -12525,11 +12525,11 @@
       </c>
       <c r="I89" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>C</v>
+        <v>B</v>
       </c>
       <c r="J89">
         <f t="shared" ca="1" si="3"/>
-        <v>0.12328010778092313</v>
+        <v>0.51627337460411538</v>
       </c>
     </row>
     <row r="90" spans="2:10" x14ac:dyDescent="0.25">
@@ -12560,7 +12560,7 @@
       </c>
       <c r="J90">
         <f t="shared" ca="1" si="3"/>
-        <v>0.89089741991058824</v>
+        <v>0.9210301064765527</v>
       </c>
     </row>
     <row r="91" spans="2:10" x14ac:dyDescent="0.25">
@@ -12587,11 +12587,11 @@
       </c>
       <c r="I91" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>C</v>
+        <v>A</v>
       </c>
       <c r="J91">
         <f t="shared" ca="1" si="3"/>
-        <v>9.7832675172202399E-2</v>
+        <v>0.86162757114661448</v>
       </c>
     </row>
     <row r="92" spans="2:10" x14ac:dyDescent="0.25">
@@ -12622,7 +12622,7 @@
       </c>
       <c r="J92">
         <f t="shared" ca="1" si="3"/>
-        <v>0.85275666046487208</v>
+        <v>0.83114356565723801</v>
       </c>
     </row>
     <row r="93" spans="2:10" x14ac:dyDescent="0.25">
@@ -12649,11 +12649,11 @@
       </c>
       <c r="I93" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>A</v>
+        <v>B</v>
       </c>
       <c r="J93">
         <f t="shared" ca="1" si="3"/>
-        <v>0.91822122663074313</v>
+        <v>0.42449206050823218</v>
       </c>
     </row>
     <row r="94" spans="2:10" x14ac:dyDescent="0.25">
@@ -12680,11 +12680,11 @@
       </c>
       <c r="I94" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>C</v>
+        <v>B</v>
       </c>
       <c r="J94">
         <f t="shared" ca="1" si="3"/>
-        <v>0.13406183340901956</v>
+        <v>0.44566565857114726</v>
       </c>
     </row>
     <row r="95" spans="2:10" x14ac:dyDescent="0.25">
@@ -12715,7 +12715,7 @@
       </c>
       <c r="J95">
         <f t="shared" ca="1" si="3"/>
-        <v>0.55008567167753164</v>
+        <v>0.76926671413161141</v>
       </c>
     </row>
     <row r="96" spans="2:10" x14ac:dyDescent="0.25">
@@ -12746,7 +12746,7 @@
       </c>
       <c r="J96">
         <f t="shared" ca="1" si="3"/>
-        <v>0.69951093617880056</v>
+        <v>0.42815196468080741</v>
       </c>
     </row>
     <row r="97" spans="2:10" x14ac:dyDescent="0.25">
@@ -12758,31 +12758,31 @@
       </c>
       <c r="D97">
         <f t="shared" ref="D97:D114" ca="1" si="4">FLOOR(RAND()*10,1)</f>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E97">
         <f t="shared" ref="E97:H114" ca="1" si="5">FLOOR(RAND()*1000,1)</f>
-        <v>259</v>
+        <v>33</v>
       </c>
       <c r="F97">
         <f t="shared" ca="1" si="5"/>
-        <v>278</v>
+        <v>690</v>
       </c>
       <c r="G97">
         <f t="shared" ca="1" si="5"/>
-        <v>155</v>
+        <v>959</v>
       </c>
       <c r="H97">
         <f t="shared" ca="1" si="5"/>
-        <v>919</v>
+        <v>740</v>
       </c>
       <c r="I97" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>C</v>
+        <v>B</v>
       </c>
       <c r="J97">
         <f t="shared" ca="1" si="3"/>
-        <v>0.20549639091819161</v>
+        <v>0.55863915446936085</v>
       </c>
     </row>
     <row r="98" spans="2:10" x14ac:dyDescent="0.25">
@@ -12794,23 +12794,23 @@
       </c>
       <c r="D98">
         <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E98">
         <f t="shared" ca="1" si="5"/>
-        <v>37</v>
+        <v>323</v>
       </c>
       <c r="F98">
         <f t="shared" ca="1" si="5"/>
-        <v>257</v>
+        <v>911</v>
       </c>
       <c r="G98">
         <f t="shared" ca="1" si="5"/>
-        <v>834</v>
+        <v>389</v>
       </c>
       <c r="H98">
         <f t="shared" ca="1" si="5"/>
-        <v>79</v>
+        <v>532</v>
       </c>
       <c r="I98" t="str">
         <f t="shared" ca="1" si="2"/>
@@ -12818,7 +12818,7 @@
       </c>
       <c r="J98">
         <f t="shared" ca="1" si="3"/>
-        <v>8.5154997316028269E-2</v>
+        <v>0.27108409256910115</v>
       </c>
     </row>
     <row r="99" spans="2:10" x14ac:dyDescent="0.25">
@@ -12830,31 +12830,31 @@
       </c>
       <c r="D99">
         <f t="shared" ca="1" si="4"/>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E99">
         <f t="shared" ca="1" si="5"/>
-        <v>748</v>
+        <v>844</v>
       </c>
       <c r="F99">
         <f t="shared" ca="1" si="5"/>
-        <v>988</v>
+        <v>307</v>
       </c>
       <c r="G99">
         <f t="shared" ca="1" si="5"/>
-        <v>552</v>
+        <v>61</v>
       </c>
       <c r="H99">
         <f t="shared" ca="1" si="5"/>
-        <v>247</v>
+        <v>140</v>
       </c>
       <c r="I99" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>C</v>
+        <v>B</v>
       </c>
       <c r="J99">
         <f t="shared" ca="1" si="3"/>
-        <v>0.26955049924018937</v>
+        <v>0.49257090122865588</v>
       </c>
     </row>
     <row r="100" spans="2:10" x14ac:dyDescent="0.25">
@@ -12866,31 +12866,31 @@
       </c>
       <c r="D100">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E100">
         <f t="shared" ca="1" si="5"/>
-        <v>307</v>
+        <v>331</v>
       </c>
       <c r="F100">
         <f t="shared" ca="1" si="5"/>
-        <v>880</v>
+        <v>0</v>
       </c>
       <c r="G100">
         <f t="shared" ca="1" si="5"/>
-        <v>282</v>
+        <v>36</v>
       </c>
       <c r="H100">
         <f t="shared" ca="1" si="5"/>
-        <v>243</v>
+        <v>975</v>
       </c>
       <c r="I100" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>C</v>
+        <v>B</v>
       </c>
       <c r="J100">
         <f t="shared" ca="1" si="3"/>
-        <v>0.21745786010587564</v>
+        <v>0.41050423020193105</v>
       </c>
     </row>
     <row r="101" spans="2:10" x14ac:dyDescent="0.25">
@@ -12902,31 +12902,31 @@
       </c>
       <c r="D101">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E101">
         <f t="shared" ca="1" si="5"/>
-        <v>345</v>
+        <v>297</v>
       </c>
       <c r="F101">
         <f t="shared" ca="1" si="5"/>
-        <v>194</v>
+        <v>79</v>
       </c>
       <c r="G101">
         <f t="shared" ca="1" si="5"/>
-        <v>475</v>
+        <v>709</v>
       </c>
       <c r="H101">
         <f t="shared" ca="1" si="5"/>
-        <v>800</v>
+        <v>585</v>
       </c>
       <c r="I101" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>B</v>
+        <v>A</v>
       </c>
       <c r="J101">
         <f t="shared" ca="1" si="3"/>
-        <v>0.42445069603536401</v>
+        <v>0.86565856183216172</v>
       </c>
     </row>
     <row r="102" spans="2:10" x14ac:dyDescent="0.25">
@@ -12938,31 +12938,31 @@
       </c>
       <c r="D102">
         <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E102">
         <f t="shared" ca="1" si="5"/>
-        <v>753</v>
+        <v>662</v>
       </c>
       <c r="F102">
         <f t="shared" ca="1" si="5"/>
-        <v>646</v>
+        <v>30</v>
       </c>
       <c r="G102">
         <f t="shared" ca="1" si="5"/>
-        <v>367</v>
+        <v>758</v>
       </c>
       <c r="H102">
         <f t="shared" ca="1" si="5"/>
-        <v>729</v>
+        <v>973</v>
       </c>
       <c r="I102" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>B</v>
+        <v>C</v>
       </c>
       <c r="J102">
         <f t="shared" ca="1" si="3"/>
-        <v>0.72676877553127284</v>
+        <v>0.20292970592418003</v>
       </c>
     </row>
     <row r="103" spans="2:10" x14ac:dyDescent="0.25">
@@ -12974,31 +12974,31 @@
       </c>
       <c r="D103">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E103">
         <f t="shared" ca="1" si="5"/>
-        <v>937</v>
+        <v>222</v>
       </c>
       <c r="F103">
         <f t="shared" ca="1" si="5"/>
-        <v>817</v>
+        <v>399</v>
       </c>
       <c r="G103">
         <f t="shared" ca="1" si="5"/>
-        <v>862</v>
+        <v>749</v>
       </c>
       <c r="H103">
         <f t="shared" ca="1" si="5"/>
-        <v>738</v>
+        <v>350</v>
       </c>
       <c r="I103" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>A</v>
+        <v>B</v>
       </c>
       <c r="J103">
         <f t="shared" ca="1" si="3"/>
-        <v>0.88512039665138587</v>
+        <v>0.30703125453414271</v>
       </c>
     </row>
     <row r="104" spans="2:10" x14ac:dyDescent="0.25">
@@ -13010,23 +13010,23 @@
       </c>
       <c r="D104">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E104">
         <f t="shared" ca="1" si="5"/>
-        <v>250</v>
+        <v>522</v>
       </c>
       <c r="F104">
         <f t="shared" ca="1" si="5"/>
-        <v>168</v>
+        <v>76</v>
       </c>
       <c r="G104">
         <f t="shared" ca="1" si="5"/>
-        <v>788</v>
+        <v>660</v>
       </c>
       <c r="H104">
         <f t="shared" ca="1" si="5"/>
-        <v>625</v>
+        <v>17</v>
       </c>
       <c r="I104" t="str">
         <f t="shared" ca="1" si="2"/>
@@ -13034,7 +13034,7 @@
       </c>
       <c r="J104">
         <f t="shared" ca="1" si="3"/>
-        <v>0.49052030580392403</v>
+        <v>0.46969970621806079</v>
       </c>
     </row>
     <row r="105" spans="2:10" x14ac:dyDescent="0.25">
@@ -13046,31 +13046,31 @@
       </c>
       <c r="D105">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E105">
         <f t="shared" ca="1" si="5"/>
-        <v>584</v>
+        <v>480</v>
       </c>
       <c r="F105">
         <f t="shared" ca="1" si="5"/>
-        <v>834</v>
+        <v>568</v>
       </c>
       <c r="G105">
         <f t="shared" ca="1" si="5"/>
-        <v>841</v>
+        <v>74</v>
       </c>
       <c r="H105">
         <f t="shared" ca="1" si="5"/>
-        <v>213</v>
+        <v>199</v>
       </c>
       <c r="I105" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>B</v>
+        <v>C</v>
       </c>
       <c r="J105">
         <f t="shared" ca="1" si="3"/>
-        <v>0.59568584258424462</v>
+        <v>6.9292364819329988E-3</v>
       </c>
     </row>
     <row r="106" spans="2:10" x14ac:dyDescent="0.25">
@@ -13082,31 +13082,31 @@
       </c>
       <c r="D106">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E106">
         <f t="shared" ca="1" si="5"/>
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="F106">
         <f t="shared" ca="1" si="5"/>
-        <v>890</v>
+        <v>825</v>
       </c>
       <c r="G106">
         <f t="shared" ca="1" si="5"/>
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="H106">
         <f t="shared" ca="1" si="5"/>
-        <v>574</v>
+        <v>371</v>
       </c>
       <c r="I106" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>B</v>
+        <v>C</v>
       </c>
       <c r="J106">
         <f t="shared" ca="1" si="3"/>
-        <v>0.53192075855856891</v>
+        <v>7.7346031061725773E-2</v>
       </c>
     </row>
     <row r="107" spans="2:10" x14ac:dyDescent="0.25">
@@ -13118,31 +13118,31 @@
       </c>
       <c r="D107">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E107">
         <f t="shared" ca="1" si="5"/>
-        <v>569</v>
+        <v>186</v>
       </c>
       <c r="F107">
         <f t="shared" ca="1" si="5"/>
-        <v>38</v>
+        <v>423</v>
       </c>
       <c r="G107">
         <f t="shared" ca="1" si="5"/>
-        <v>493</v>
+        <v>792</v>
       </c>
       <c r="H107">
         <f t="shared" ca="1" si="5"/>
-        <v>956</v>
+        <v>901</v>
       </c>
       <c r="I107" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>C</v>
+        <v>B</v>
       </c>
       <c r="J107">
         <f t="shared" ca="1" si="3"/>
-        <v>1.3045638784383806E-2</v>
+        <v>0.43480758454005219</v>
       </c>
     </row>
     <row r="108" spans="2:10" x14ac:dyDescent="0.25">
@@ -13154,23 +13154,23 @@
       </c>
       <c r="D108">
         <f t="shared" ca="1" si="4"/>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E108">
         <f t="shared" ca="1" si="5"/>
-        <v>796</v>
+        <v>455</v>
       </c>
       <c r="F108">
         <f t="shared" ca="1" si="5"/>
-        <v>772</v>
+        <v>179</v>
       </c>
       <c r="G108">
         <f t="shared" ca="1" si="5"/>
-        <v>533</v>
+        <v>676</v>
       </c>
       <c r="H108">
         <f t="shared" ca="1" si="5"/>
-        <v>767</v>
+        <v>117</v>
       </c>
       <c r="I108" t="str">
         <f t="shared" ca="1" si="2"/>
@@ -13178,7 +13178,7 @@
       </c>
       <c r="J108">
         <f t="shared" ca="1" si="3"/>
-        <v>0.91844696492719347</v>
+        <v>0.90878750661967178</v>
       </c>
     </row>
     <row r="109" spans="2:10" x14ac:dyDescent="0.25">
@@ -13190,23 +13190,23 @@
       </c>
       <c r="D109">
         <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E109">
         <f t="shared" ca="1" si="5"/>
-        <v>983</v>
+        <v>474</v>
       </c>
       <c r="F109">
         <f t="shared" ca="1" si="5"/>
-        <v>212</v>
+        <v>882</v>
       </c>
       <c r="G109">
         <f t="shared" ca="1" si="5"/>
-        <v>705</v>
+        <v>233</v>
       </c>
       <c r="H109">
         <f t="shared" ca="1" si="5"/>
-        <v>518</v>
+        <v>637</v>
       </c>
       <c r="I109" t="str">
         <f t="shared" ca="1" si="2"/>
@@ -13214,7 +13214,7 @@
       </c>
       <c r="J109">
         <f t="shared" ca="1" si="3"/>
-        <v>0.99053056535836359</v>
+        <v>0.95514670370301968</v>
       </c>
     </row>
     <row r="110" spans="2:10" x14ac:dyDescent="0.25">
@@ -13226,31 +13226,31 @@
       </c>
       <c r="D110">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E110">
         <f t="shared" ca="1" si="5"/>
-        <v>867</v>
+        <v>415</v>
       </c>
       <c r="F110">
         <f t="shared" ca="1" si="5"/>
-        <v>82</v>
+        <v>760</v>
       </c>
       <c r="G110">
         <f t="shared" ca="1" si="5"/>
-        <v>443</v>
+        <v>899</v>
       </c>
       <c r="H110">
         <f t="shared" ca="1" si="5"/>
-        <v>905</v>
+        <v>931</v>
       </c>
       <c r="I110" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>A</v>
+        <v>B</v>
       </c>
       <c r="J110">
         <f t="shared" ca="1" si="3"/>
-        <v>0.85005379251428437</v>
+        <v>0.63815614114002339</v>
       </c>
     </row>
     <row r="111" spans="2:10" x14ac:dyDescent="0.25">
@@ -13262,23 +13262,23 @@
       </c>
       <c r="D111">
         <f t="shared" ca="1" si="4"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E111">
         <f t="shared" ca="1" si="5"/>
-        <v>623</v>
+        <v>852</v>
       </c>
       <c r="F111">
         <f t="shared" ca="1" si="5"/>
-        <v>366</v>
+        <v>196</v>
       </c>
       <c r="G111">
         <f t="shared" ca="1" si="5"/>
-        <v>65</v>
+        <v>816</v>
       </c>
       <c r="H111">
         <f t="shared" ca="1" si="5"/>
-        <v>601</v>
+        <v>240</v>
       </c>
       <c r="I111" t="str">
         <f t="shared" ca="1" si="2"/>
@@ -13286,7 +13286,7 @@
       </c>
       <c r="J111">
         <f t="shared" ca="1" si="3"/>
-        <v>0.58610667789520887</v>
+        <v>0.61039766012656926</v>
       </c>
     </row>
     <row r="112" spans="2:10" x14ac:dyDescent="0.25">
@@ -13298,31 +13298,31 @@
       </c>
       <c r="D112">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E112">
         <f t="shared" ca="1" si="5"/>
-        <v>655</v>
+        <v>917</v>
       </c>
       <c r="F112">
         <f t="shared" ca="1" si="5"/>
-        <v>450</v>
+        <v>178</v>
       </c>
       <c r="G112">
         <f t="shared" ca="1" si="5"/>
-        <v>876</v>
+        <v>551</v>
       </c>
       <c r="H112">
         <f t="shared" ca="1" si="5"/>
-        <v>280</v>
+        <v>222</v>
       </c>
       <c r="I112" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>C</v>
+        <v>B</v>
       </c>
       <c r="J112">
         <f t="shared" ca="1" si="3"/>
-        <v>5.371243846451268E-2</v>
+        <v>0.63282954449651285</v>
       </c>
     </row>
     <row r="113" spans="2:10" x14ac:dyDescent="0.25">
@@ -13338,27 +13338,27 @@
       </c>
       <c r="E113">
         <f t="shared" ca="1" si="5"/>
-        <v>438</v>
+        <v>955</v>
       </c>
       <c r="F113">
         <f t="shared" ca="1" si="5"/>
-        <v>445</v>
+        <v>173</v>
       </c>
       <c r="G113">
         <f t="shared" ca="1" si="5"/>
-        <v>457</v>
+        <v>159</v>
       </c>
       <c r="H113">
         <f t="shared" ca="1" si="5"/>
-        <v>101</v>
+        <v>803</v>
       </c>
       <c r="I113" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>C</v>
+        <v>A</v>
       </c>
       <c r="J113">
         <f t="shared" ca="1" si="3"/>
-        <v>0.1284463086913592</v>
+        <v>0.80924421576687988</v>
       </c>
     </row>
     <row r="114" spans="2:10" x14ac:dyDescent="0.25">
@@ -13370,31 +13370,31 @@
       </c>
       <c r="D114">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E114">
         <f t="shared" ca="1" si="5"/>
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="F114">
         <f t="shared" ca="1" si="5"/>
-        <v>873</v>
+        <v>210</v>
       </c>
       <c r="G114">
         <f t="shared" ca="1" si="5"/>
-        <v>293</v>
+        <v>710</v>
       </c>
       <c r="H114">
         <f t="shared" ca="1" si="5"/>
-        <v>471</v>
+        <v>304</v>
       </c>
       <c r="I114" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>B</v>
+        <v>C</v>
       </c>
       <c r="J114">
         <f t="shared" ca="1" si="3"/>
-        <v>0.42094205823284148</v>
+        <v>9.2114147748910025E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>